<commit_message>
Modificati tassi di uscita OPTN. Risolto problema con i tassi totali.
</commit_message>
<xml_diff>
--- a/data/Data_Tansplants_US.xlsx
+++ b/data/Data_Tansplants_US.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FF5F932-9BFF-4885-A88C-3890130FC173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE0926EB-6D89-467C-841C-300FA50C6DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="67">
   <si>
     <t>ORGANI</t>
   </si>
@@ -216,9 +216,6 @@
     <t>TRAPIANTI</t>
   </si>
   <si>
-    <t>NCS</t>
-  </si>
-  <si>
     <t>PROBABILITÀ - USCITE</t>
   </si>
   <si>
@@ -313,21 +310,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -407,48 +398,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -520,13 +474,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -846,12 +799,13 @@
   </sheetPr>
   <dimension ref="A1:AO237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="M116" sqref="M116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="29" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -8667,11 +8621,9 @@
       <c r="F113" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G113" s="35" t="s">
+      <c r="G113" s="31"/>
+      <c r="I113" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="I113" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="J113" s="20"/>
       <c r="K113" s="9" t="s">
@@ -8690,37 +8642,26 @@
       </c>
       <c r="C114" s="6">
         <f>AVERAGE(L138:Q138)</f>
-        <v>31352.666666666668</v>
-      </c>
-      <c r="D114" s="31">
+        <v>32282.833333333332</v>
+      </c>
+      <c r="D114" s="32">
         <f>AVERAGE(M206:R206)</f>
-        <v>4708</v>
+        <v>4787</v>
       </c>
       <c r="E114" s="6">
         <f>C114-D114-F114</f>
-        <v>14937.833333333334</v>
+        <v>15788.666666666666</v>
       </c>
       <c r="F114" s="6">
         <f>AVERAGE(M172:R172)</f>
-        <v>11706.833333333334</v>
-      </c>
-      <c r="G114" s="32">
-        <f>D115+D116+D117</f>
-        <v>4787</v>
-      </c>
+        <v>11707.166666666666</v>
+      </c>
+      <c r="G114" s="33"/>
       <c r="I114" t="s">
         <v>3</v>
       </c>
       <c r="J114" t="s">
         <v>9</v>
-      </c>
-      <c r="K114">
-        <f>K118+K122+K126+K130</f>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="L114">
-        <f>L118+L122+L126+L130</f>
-        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="115" spans="1:13">
@@ -8743,20 +8684,9 @@
         <f>SUM(AVERAGE(M186:R186),AVERAGE(M191:R191))</f>
         <v>20.833333333333332</v>
       </c>
-      <c r="G115" s="33">
-        <f>SUM(AVERAGE(M220:R220),AVERAGE(M225:R225))</f>
-        <v>2.8333333333333335</v>
-      </c>
+      <c r="G115" s="34"/>
       <c r="J115" t="s">
         <v>16</v>
-      </c>
-      <c r="K115">
-        <f>K119+K123+K127+K131</f>
-        <v>1</v>
-      </c>
-      <c r="L115">
-        <f>L119+L123+L127+L131</f>
-        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="116" spans="1:13">
@@ -8779,20 +8709,9 @@
         <f>SUM(AVERAGE(M177:R177),AVERAGE(M181:R181))</f>
         <v>11679.666666666666</v>
       </c>
-      <c r="G116" s="33">
-        <f>SUM(AVERAGE(M211:R211),AVERAGE(M215:R215))</f>
-        <v>1785.3333333333333</v>
-      </c>
+      <c r="G116" s="34"/>
       <c r="J116" t="s">
         <v>17</v>
-      </c>
-      <c r="K116">
-        <f>K120+K124+K128+K132</f>
-        <v>1</v>
-      </c>
-      <c r="L116">
-        <f>L120+L124+L128+L132</f>
-        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:13">
@@ -8815,20 +8734,9 @@
         <f>AVERAGE(M196:R196)</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="G117" s="34">
-        <f>AVERAGE(M230:R230)</f>
-        <v>2998.8333333333335</v>
-      </c>
+      <c r="G117" s="34"/>
       <c r="J117" t="s">
         <v>18</v>
-      </c>
-      <c r="K117">
-        <f>K121+K125+K129+K133</f>
-        <v>1</v>
-      </c>
-      <c r="L117">
-        <f>L121+L125+L129+L133</f>
-        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="118" spans="1:13">
@@ -8840,15 +8748,15 @@
       </c>
       <c r="C118" s="6">
         <f>AVERAGE(L139:Q139)</f>
-        <v>15034.5</v>
+        <v>15490.5</v>
       </c>
       <c r="D118" s="6">
         <f>AVERAGE(M207:R207)</f>
-        <v>2431.6666666666665</v>
+        <v>2477.1666666666665</v>
       </c>
       <c r="E118" s="6">
         <f>C118-D118-F118</f>
-        <v>7259.0000000000009</v>
+        <v>7669.5000000000009</v>
       </c>
       <c r="F118" s="6">
         <f>AVERAGE(M173:R173)</f>
@@ -8863,11 +8771,11 @@
       </c>
       <c r="K118">
         <f>D118/D114</f>
-        <v>0.51649674313225713</v>
+        <v>0.51747789151173318</v>
       </c>
       <c r="L118">
         <f>E118/E114</f>
-        <v>0.4859473149832082</v>
+        <v>0.48575982772452819</v>
       </c>
     </row>
     <row r="119" spans="1:13">
@@ -8975,20 +8883,21 @@
       </c>
       <c r="C122" s="6">
         <f>AVERAGE(L140:Q140)</f>
-        <v>10557.833333333334</v>
+        <v>10862.333333333334</v>
       </c>
       <c r="D122" s="6">
         <f>AVERAGE(M208:R208)</f>
-        <v>1396.8333333333333</v>
+        <v>1413.8333333333333</v>
       </c>
       <c r="E122" s="6">
         <f t="shared" si="30"/>
-        <v>4959.166666666667</v>
+        <v>5246.333333333333</v>
       </c>
       <c r="F122" s="6">
         <f>AVERAGE(M174:R174)</f>
-        <v>4201.833333333333</v>
-      </c>
+        <v>4202.166666666667</v>
+      </c>
+      <c r="G122" s="6"/>
       <c r="I122" t="s">
         <v>5</v>
       </c>
@@ -8997,11 +8906,11 @@
       </c>
       <c r="K122">
         <f>D122/D114</f>
-        <v>0.29669357122628148</v>
+        <v>0.295348513334726</v>
       </c>
       <c r="L122">
         <f>E122/E114</f>
-        <v>0.33198701284211229</v>
+        <v>0.3322847612211291</v>
       </c>
     </row>
     <row r="123" spans="1:13">
@@ -9109,20 +9018,21 @@
       </c>
       <c r="C126" s="6">
         <f>AVERAGE(L141:Q141)</f>
-        <v>4504</v>
+        <v>4636.666666666667</v>
       </c>
       <c r="D126" s="6">
         <f>AVERAGE(M209:R209)</f>
-        <v>743.33333333333337</v>
+        <v>758.66666666666663</v>
       </c>
       <c r="E126" s="6">
         <f t="shared" si="30"/>
-        <v>2218.333333333333</v>
+        <v>2335.666666666667</v>
       </c>
       <c r="F126" s="6">
         <f>AVERAGE(M175:R175)</f>
         <v>1542.3333333333333</v>
       </c>
+      <c r="G126" s="6"/>
       <c r="I126" t="s">
         <v>6</v>
       </c>
@@ -9131,11 +9041,11 @@
       </c>
       <c r="K126">
         <f>D126/D114</f>
-        <v>0.15788728405550836</v>
+        <v>0.15848478518209039</v>
       </c>
       <c r="L126">
         <f>E126/E114</f>
-        <v>0.14850435694600955</v>
+        <v>0.1479331165815142</v>
       </c>
     </row>
     <row r="127" spans="1:13">
@@ -9244,20 +9154,21 @@
       </c>
       <c r="C130" s="6">
         <f>AVERAGE(L142:Q142)</f>
-        <v>1256.3333333333333</v>
+        <v>1293.3333333333333</v>
       </c>
       <c r="D130" s="6">
         <f>AVERAGE(M210:R210)</f>
-        <v>136.16666666666666</v>
+        <v>137.33333333333334</v>
       </c>
       <c r="E130" s="6">
         <f>C130-D130-F130</f>
-        <v>501.33333333333314</v>
+        <v>537.16666666666663</v>
       </c>
       <c r="F130" s="6">
         <f>AVERAGE(M176:R176)</f>
         <v>618.83333333333337</v>
       </c>
+      <c r="G130" s="6"/>
       <c r="I130" t="s">
         <v>7</v>
       </c>
@@ -9266,11 +9177,11 @@
       </c>
       <c r="K130">
         <f>D130/D114</f>
-        <v>2.8922401585952984E-2</v>
+        <v>2.8688809971450457E-2</v>
       </c>
       <c r="L130">
         <f>E130/E114</f>
-        <v>3.3561315228669918E-2</v>
+        <v>3.4022294472828611E-2</v>
       </c>
     </row>
     <row r="131" spans="1:35">
@@ -9373,7 +9284,10 @@
       <c r="C134" s="5"/>
     </row>
     <row r="135" spans="1:35">
+      <c r="H135" s="4"/>
+      <c r="I135" s="4"/>
       <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
       <c r="L135" s="4"/>
       <c r="M135" s="4"/>
       <c r="N135" s="4"/>
@@ -9391,7 +9305,7 @@
     </row>
     <row r="137" spans="1:35">
       <c r="A137" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B137" s="17"/>
       <c r="D137" s="1" t="s">
@@ -9495,123 +9409,123 @@
       <c r="C138" s="1"/>
       <c r="D138" s="3">
         <f>D139+D140+D141+D142</f>
-        <v>660539</v>
+        <v>715213</v>
       </c>
       <c r="E138" s="3">
         <f t="shared" ref="E138:AG138" si="31">E139+E140+E141+E142</f>
-        <v>17597</v>
+        <v>18134</v>
       </c>
       <c r="F138" s="3">
         <f t="shared" si="31"/>
-        <v>40032</v>
+        <v>41364</v>
       </c>
       <c r="G138" s="3">
         <f t="shared" si="31"/>
-        <v>38719</v>
+        <v>40012</v>
       </c>
       <c r="H138" s="3">
         <f t="shared" si="31"/>
-        <v>36976</v>
+        <v>38135</v>
       </c>
       <c r="I138" s="3">
         <f t="shared" si="31"/>
-        <v>38208</v>
+        <v>39384</v>
       </c>
       <c r="J138" s="3">
         <f t="shared" si="31"/>
-        <v>36616</v>
+        <v>37718</v>
       </c>
       <c r="K138" s="3">
         <f t="shared" si="31"/>
-        <v>35805</v>
+        <v>36883</v>
       </c>
       <c r="L138" s="3">
         <f t="shared" si="31"/>
-        <v>35255</v>
+        <v>36340</v>
       </c>
       <c r="M138" s="3">
         <f t="shared" si="31"/>
-        <v>33964</v>
+        <v>35014</v>
       </c>
       <c r="N138" s="3">
         <f t="shared" si="31"/>
-        <v>31403</v>
+        <v>32353</v>
       </c>
       <c r="O138" s="3">
         <f t="shared" si="31"/>
-        <v>29921</v>
+        <v>30809</v>
       </c>
       <c r="P138" s="3">
         <f t="shared" si="31"/>
-        <v>28866</v>
+        <v>29685</v>
       </c>
       <c r="Q138" s="3">
         <f t="shared" si="31"/>
-        <v>28707</v>
+        <v>29496</v>
       </c>
       <c r="R138" s="3">
         <f t="shared" si="31"/>
-        <v>27802</v>
+        <v>28537</v>
       </c>
       <c r="S138" s="3">
         <f t="shared" si="31"/>
-        <v>27104</v>
+        <v>27783</v>
       </c>
       <c r="T138" s="3">
         <f t="shared" si="31"/>
-        <v>26745</v>
+        <v>27444</v>
       </c>
       <c r="U138" s="3">
         <f t="shared" si="31"/>
-        <v>25876</v>
+        <v>26476</v>
       </c>
       <c r="V138" s="3">
         <f t="shared" si="31"/>
-        <v>25389</v>
+        <v>25885</v>
       </c>
       <c r="W138" s="3">
         <f t="shared" si="31"/>
-        <v>24185</v>
+        <v>24644</v>
       </c>
       <c r="X138" s="3">
         <f t="shared" si="31"/>
-        <v>21944</v>
+        <v>22297</v>
       </c>
       <c r="Y138" s="3">
         <f t="shared" si="31"/>
-        <v>20597</v>
+        <v>20810</v>
       </c>
       <c r="Z138" s="3">
         <f t="shared" si="31"/>
-        <v>20133</v>
+        <v>20368</v>
       </c>
       <c r="AA138" s="3">
         <f t="shared" si="31"/>
-        <v>18915</v>
+        <v>19116</v>
       </c>
       <c r="AB138" s="3">
         <f t="shared" si="31"/>
-        <v>18286</v>
+        <v>18523</v>
       </c>
       <c r="AC138" s="3">
         <f t="shared" si="31"/>
-        <v>17252</v>
+        <v>17390</v>
       </c>
       <c r="AD138" s="3">
         <f t="shared" si="31"/>
-        <v>15725</v>
+        <v>15855</v>
       </c>
       <c r="AE138" s="3">
         <f t="shared" si="31"/>
-        <v>14621</v>
+        <v>14754</v>
       </c>
       <c r="AF138" s="3">
         <f t="shared" si="31"/>
-        <v>13942</v>
+        <v>14081</v>
       </c>
       <c r="AG138" s="3">
         <f t="shared" si="31"/>
-        <v>13547</v>
+        <v>13671</v>
       </c>
     </row>
     <row r="139" spans="1:35">
@@ -9621,94 +9535,124 @@
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="3">
-        <v>314605</v>
+        <f>SUM(D144,D149,D154,D159,D164)</f>
+        <v>341845</v>
       </c>
       <c r="E139" s="3">
-        <v>8575</v>
+        <f t="shared" ref="E139:AG139" si="32">SUM(E144,E149,E154,E159,E164)</f>
+        <v>8857</v>
       </c>
       <c r="F139" s="3">
-        <v>19336</v>
+        <f t="shared" si="32"/>
+        <v>19997</v>
       </c>
       <c r="G139" s="3">
-        <v>18781</v>
+        <f t="shared" si="32"/>
+        <v>19448</v>
       </c>
       <c r="H139" s="3">
-        <v>17845</v>
+        <f t="shared" si="32"/>
+        <v>18423</v>
       </c>
       <c r="I139" s="3">
-        <v>18432</v>
+        <f t="shared" si="32"/>
+        <v>19011</v>
       </c>
       <c r="J139" s="3">
-        <v>17616</v>
+        <f t="shared" si="32"/>
+        <v>18174</v>
       </c>
       <c r="K139" s="3">
-        <v>17269</v>
+        <f t="shared" si="32"/>
+        <v>17808</v>
       </c>
       <c r="L139" s="3">
-        <v>17020</v>
+        <f t="shared" si="32"/>
+        <v>17564</v>
       </c>
       <c r="M139" s="3">
-        <v>16392</v>
+        <f t="shared" si="32"/>
+        <v>16886</v>
       </c>
       <c r="N139" s="3">
-        <v>15034</v>
+        <f t="shared" si="32"/>
+        <v>15506</v>
       </c>
       <c r="O139" s="3">
-        <v>14327</v>
+        <f t="shared" si="32"/>
+        <v>14761</v>
       </c>
       <c r="P139" s="3">
-        <v>13733</v>
+        <f t="shared" si="32"/>
+        <v>14117</v>
       </c>
       <c r="Q139" s="3">
-        <v>13701</v>
+        <f t="shared" si="32"/>
+        <v>14109</v>
       </c>
       <c r="R139" s="3">
-        <v>13369</v>
+        <f t="shared" si="32"/>
+        <v>13738</v>
       </c>
       <c r="S139" s="3">
-        <v>13068</v>
+        <f t="shared" si="32"/>
+        <v>13399</v>
       </c>
       <c r="T139" s="3">
-        <v>12714</v>
+        <f t="shared" si="32"/>
+        <v>13053</v>
       </c>
       <c r="U139" s="3">
-        <v>12452</v>
+        <f t="shared" si="32"/>
+        <v>12759</v>
       </c>
       <c r="V139" s="3">
-        <v>12056</v>
+        <f t="shared" si="32"/>
+        <v>12312</v>
       </c>
       <c r="W139" s="3">
-        <v>11495</v>
+        <f t="shared" si="32"/>
+        <v>11719</v>
       </c>
       <c r="X139" s="3">
-        <v>10511</v>
+        <f t="shared" si="32"/>
+        <v>10688</v>
       </c>
       <c r="Y139" s="3">
-        <v>9915</v>
+        <f t="shared" si="32"/>
+        <v>10027</v>
       </c>
       <c r="Z139" s="3">
-        <v>9599</v>
+        <f t="shared" si="32"/>
+        <v>9702</v>
       </c>
       <c r="AA139" s="3">
-        <v>8942</v>
+        <f t="shared" si="32"/>
+        <v>9046</v>
       </c>
       <c r="AB139" s="3">
-        <v>8691</v>
+        <f t="shared" si="32"/>
+        <v>8812</v>
       </c>
       <c r="AC139" s="3">
-        <v>7997</v>
+        <f t="shared" si="32"/>
+        <v>8070</v>
       </c>
       <c r="AD139" s="3">
-        <v>7417</v>
+        <f t="shared" si="32"/>
+        <v>7476</v>
       </c>
       <c r="AE139" s="3">
-        <v>6804</v>
+        <f t="shared" si="32"/>
+        <v>6874</v>
       </c>
       <c r="AF139" s="3">
-        <v>6458</v>
+        <f t="shared" si="32"/>
+        <v>6525</v>
       </c>
       <c r="AG139" s="3">
-        <v>6307</v>
+        <f t="shared" si="32"/>
+        <v>6365</v>
       </c>
     </row>
     <row r="140" spans="1:35">
@@ -9718,94 +9662,124 @@
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="3">
-        <v>224273</v>
+        <f>SUM(D145,D150,D155,D160,D165)</f>
+        <v>241421</v>
       </c>
       <c r="E140" s="3">
-        <v>5661</v>
+        <f t="shared" ref="E140:AG140" si="33">SUM(E145,E150,E155,E160,E165)</f>
+        <v>5835</v>
       </c>
       <c r="F140" s="3">
-        <v>12980</v>
+        <f t="shared" si="33"/>
+        <v>13388</v>
       </c>
       <c r="G140" s="3">
-        <v>12656</v>
+        <f t="shared" si="33"/>
+        <v>13017</v>
       </c>
       <c r="H140" s="3">
-        <v>12197</v>
+        <f t="shared" si="33"/>
+        <v>12573</v>
       </c>
       <c r="I140" s="3">
-        <v>12573</v>
+        <f t="shared" si="33"/>
+        <v>12934</v>
       </c>
       <c r="J140" s="3">
-        <v>12041</v>
+        <f t="shared" si="33"/>
+        <v>12379</v>
       </c>
       <c r="K140" s="3">
-        <v>11874</v>
+        <f t="shared" si="33"/>
+        <v>12202</v>
       </c>
       <c r="L140" s="3">
-        <v>11818</v>
+        <f t="shared" si="33"/>
+        <v>12175</v>
       </c>
       <c r="M140" s="3">
-        <v>11209</v>
+        <f t="shared" si="33"/>
+        <v>11557</v>
       </c>
       <c r="N140" s="3">
-        <v>10645</v>
+        <f t="shared" si="33"/>
+        <v>10963</v>
       </c>
       <c r="O140" s="3">
-        <v>10116</v>
+        <f t="shared" si="33"/>
+        <v>10400</v>
       </c>
       <c r="P140" s="3">
-        <v>9808</v>
+        <f t="shared" si="33"/>
+        <v>10078</v>
       </c>
       <c r="Q140" s="3">
-        <v>9751</v>
+        <f t="shared" si="33"/>
+        <v>10001</v>
       </c>
       <c r="R140" s="3">
-        <v>9224</v>
+        <f t="shared" si="33"/>
+        <v>9457</v>
       </c>
       <c r="S140" s="3">
-        <v>9146</v>
+        <f t="shared" si="33"/>
+        <v>9374</v>
       </c>
       <c r="T140" s="3">
-        <v>9013</v>
+        <f t="shared" si="33"/>
+        <v>9238</v>
       </c>
       <c r="U140" s="3">
-        <v>8671</v>
+        <f t="shared" si="33"/>
+        <v>8855</v>
       </c>
       <c r="V140" s="3">
-        <v>8630</v>
+        <f t="shared" si="33"/>
+        <v>8791</v>
       </c>
       <c r="W140" s="3">
-        <v>8229</v>
+        <f t="shared" si="33"/>
+        <v>8389</v>
       </c>
       <c r="X140" s="3">
-        <v>7451</v>
+        <f t="shared" si="33"/>
+        <v>7569</v>
       </c>
       <c r="Y140" s="3">
-        <v>7000</v>
+        <f t="shared" si="33"/>
+        <v>7059</v>
       </c>
       <c r="Z140" s="3">
-        <v>6907</v>
+        <f t="shared" si="33"/>
+        <v>6989</v>
       </c>
       <c r="AA140" s="3">
-        <v>6587</v>
+        <f t="shared" si="33"/>
+        <v>6652</v>
       </c>
       <c r="AB140" s="3">
-        <v>6382</v>
+        <f t="shared" si="33"/>
+        <v>6457</v>
       </c>
       <c r="AC140" s="3">
-        <v>6040</v>
+        <f t="shared" si="33"/>
+        <v>6083</v>
       </c>
       <c r="AD140" s="3">
-        <v>5485</v>
+        <f t="shared" si="33"/>
+        <v>5527</v>
       </c>
       <c r="AE140" s="3">
-        <v>5219</v>
+        <f t="shared" si="33"/>
+        <v>5260</v>
       </c>
       <c r="AF140" s="3">
-        <v>5118</v>
+        <f t="shared" si="33"/>
+        <v>5169</v>
       </c>
       <c r="AG140" s="3">
-        <v>4808</v>
+        <f t="shared" si="33"/>
+        <v>4847</v>
       </c>
       <c r="AH140" s="1"/>
       <c r="AI140" s="1"/>
@@ -9817,94 +9791,124 @@
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="3">
-        <v>94850</v>
+        <f>SUM(D146,D151,D156,D161,D166)</f>
+        <v>103252</v>
       </c>
       <c r="E141" s="3">
-        <v>2666</v>
+        <f t="shared" ref="E141:AG141" si="34">SUM(E146,E151,E156,E161,E166)</f>
+        <v>2736</v>
       </c>
       <c r="F141" s="3">
-        <v>6157</v>
+        <f t="shared" si="34"/>
+        <v>6370</v>
       </c>
       <c r="G141" s="3">
-        <v>5818</v>
+        <f t="shared" si="34"/>
+        <v>6038</v>
       </c>
       <c r="H141" s="3">
-        <v>5499</v>
+        <f t="shared" si="34"/>
+        <v>5667</v>
       </c>
       <c r="I141" s="3">
-        <v>5654</v>
+        <f t="shared" si="34"/>
+        <v>5850</v>
       </c>
       <c r="J141" s="3">
-        <v>5509</v>
+        <f t="shared" si="34"/>
+        <v>5684</v>
       </c>
       <c r="K141" s="3">
-        <v>5250</v>
+        <f t="shared" si="34"/>
+        <v>5425</v>
       </c>
       <c r="L141" s="3">
-        <v>5099</v>
+        <f t="shared" si="34"/>
+        <v>5242</v>
       </c>
       <c r="M141" s="3">
-        <v>4942</v>
+        <f t="shared" si="34"/>
+        <v>5106</v>
       </c>
       <c r="N141" s="3">
-        <v>4507</v>
+        <f t="shared" si="34"/>
+        <v>4630</v>
       </c>
       <c r="O141" s="3">
-        <v>4268</v>
+        <f t="shared" si="34"/>
+        <v>4401</v>
       </c>
       <c r="P141" s="3">
-        <v>4122</v>
+        <f t="shared" si="34"/>
+        <v>4250</v>
       </c>
       <c r="Q141" s="3">
-        <v>4086</v>
+        <f t="shared" si="34"/>
+        <v>4191</v>
       </c>
       <c r="R141" s="3">
-        <v>4059</v>
+        <f t="shared" si="34"/>
+        <v>4175</v>
       </c>
       <c r="S141" s="3">
-        <v>3811</v>
+        <f t="shared" si="34"/>
+        <v>3898</v>
       </c>
       <c r="T141" s="3">
-        <v>3955</v>
+        <f t="shared" si="34"/>
+        <v>4060</v>
       </c>
       <c r="U141" s="3">
-        <v>3683</v>
+        <f t="shared" si="34"/>
+        <v>3771</v>
       </c>
       <c r="V141" s="3">
-        <v>3635</v>
+        <f t="shared" si="34"/>
+        <v>3700</v>
       </c>
       <c r="W141" s="3">
-        <v>3495</v>
+        <f t="shared" si="34"/>
+        <v>3562</v>
       </c>
       <c r="X141" s="3">
-        <v>3115</v>
+        <f t="shared" si="34"/>
+        <v>3161</v>
       </c>
       <c r="Y141" s="3">
-        <v>2878</v>
+        <f t="shared" si="34"/>
+        <v>2917</v>
       </c>
       <c r="Z141" s="3">
-        <v>2820</v>
+        <f t="shared" si="34"/>
+        <v>2865</v>
       </c>
       <c r="AA141" s="3">
-        <v>2624</v>
+        <f t="shared" si="34"/>
+        <v>2655</v>
       </c>
       <c r="AB141" s="3">
-        <v>2501</v>
+        <f t="shared" si="34"/>
+        <v>2536</v>
       </c>
       <c r="AC141" s="3">
-        <v>2464</v>
+        <f t="shared" si="34"/>
+        <v>2482</v>
       </c>
       <c r="AD141" s="3">
-        <v>2196</v>
+        <f t="shared" si="34"/>
+        <v>2221</v>
       </c>
       <c r="AE141" s="3">
-        <v>2006</v>
+        <f t="shared" si="34"/>
+        <v>2023</v>
       </c>
       <c r="AF141" s="3">
-        <v>1791</v>
+        <f t="shared" si="34"/>
+        <v>1807</v>
       </c>
       <c r="AG141" s="3">
-        <v>1839</v>
+        <f t="shared" si="34"/>
+        <v>1859</v>
       </c>
       <c r="AH141" s="1"/>
       <c r="AI141" s="1"/>
@@ -9916,94 +9920,124 @@
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="3">
-        <v>26811</v>
-      </c>
-      <c r="E142" s="1">
-        <v>695</v>
+        <f>SUM(D147,D152,D157,D162,D167)</f>
+        <v>28695</v>
+      </c>
+      <c r="E142" s="3">
+        <f t="shared" ref="E142:AG142" si="35">SUM(E147,E152,E157,E162,E167)</f>
+        <v>706</v>
       </c>
       <c r="F142" s="3">
-        <v>1559</v>
+        <f t="shared" si="35"/>
+        <v>1609</v>
       </c>
       <c r="G142" s="3">
-        <v>1464</v>
+        <f t="shared" si="35"/>
+        <v>1509</v>
       </c>
       <c r="H142" s="3">
-        <v>1435</v>
+        <f t="shared" si="35"/>
+        <v>1472</v>
       </c>
       <c r="I142" s="3">
-        <v>1549</v>
+        <f t="shared" si="35"/>
+        <v>1589</v>
       </c>
       <c r="J142" s="3">
-        <v>1450</v>
+        <f t="shared" si="35"/>
+        <v>1481</v>
       </c>
       <c r="K142" s="3">
-        <v>1412</v>
+        <f t="shared" si="35"/>
+        <v>1448</v>
       </c>
       <c r="L142" s="3">
-        <v>1318</v>
+        <f t="shared" si="35"/>
+        <v>1359</v>
       </c>
       <c r="M142" s="3">
-        <v>1421</v>
+        <f t="shared" si="35"/>
+        <v>1465</v>
       </c>
       <c r="N142" s="3">
-        <v>1217</v>
+        <f t="shared" si="35"/>
+        <v>1254</v>
       </c>
       <c r="O142" s="3">
-        <v>1210</v>
+        <f t="shared" si="35"/>
+        <v>1247</v>
       </c>
       <c r="P142" s="3">
-        <v>1203</v>
+        <f t="shared" si="35"/>
+        <v>1240</v>
       </c>
       <c r="Q142" s="3">
-        <v>1169</v>
+        <f t="shared" si="35"/>
+        <v>1195</v>
       </c>
       <c r="R142" s="3">
-        <v>1150</v>
+        <f t="shared" si="35"/>
+        <v>1167</v>
       </c>
       <c r="S142" s="3">
-        <v>1079</v>
+        <f t="shared" si="35"/>
+        <v>1112</v>
       </c>
       <c r="T142" s="3">
-        <v>1063</v>
+        <f t="shared" si="35"/>
+        <v>1093</v>
       </c>
       <c r="U142" s="3">
-        <v>1070</v>
+        <f t="shared" si="35"/>
+        <v>1091</v>
       </c>
       <c r="V142" s="3">
-        <v>1068</v>
-      </c>
-      <c r="W142" s="1">
-        <v>966</v>
-      </c>
-      <c r="X142" s="1">
-        <v>867</v>
-      </c>
-      <c r="Y142" s="1">
-        <v>804</v>
-      </c>
-      <c r="Z142" s="1">
+        <f t="shared" si="35"/>
+        <v>1082</v>
+      </c>
+      <c r="W142" s="3">
+        <f t="shared" si="35"/>
+        <v>974</v>
+      </c>
+      <c r="X142" s="3">
+        <f t="shared" si="35"/>
+        <v>879</v>
+      </c>
+      <c r="Y142" s="3">
+        <f t="shared" si="35"/>
         <v>807</v>
       </c>
-      <c r="AA142" s="1">
-        <v>762</v>
-      </c>
-      <c r="AB142" s="1">
-        <v>712</v>
-      </c>
-      <c r="AC142" s="1">
-        <v>751</v>
-      </c>
-      <c r="AD142" s="1">
-        <v>627</v>
-      </c>
-      <c r="AE142" s="1">
-        <v>592</v>
-      </c>
-      <c r="AF142" s="1">
-        <v>575</v>
-      </c>
-      <c r="AG142" s="1">
-        <v>593</v>
+      <c r="Z142" s="3">
+        <f t="shared" si="35"/>
+        <v>812</v>
+      </c>
+      <c r="AA142" s="3">
+        <f t="shared" si="35"/>
+        <v>763</v>
+      </c>
+      <c r="AB142" s="3">
+        <f t="shared" si="35"/>
+        <v>718</v>
+      </c>
+      <c r="AC142" s="3">
+        <f t="shared" si="35"/>
+        <v>755</v>
+      </c>
+      <c r="AD142" s="3">
+        <f t="shared" si="35"/>
+        <v>631</v>
+      </c>
+      <c r="AE142" s="3">
+        <f t="shared" si="35"/>
+        <v>597</v>
+      </c>
+      <c r="AF142" s="3">
+        <f t="shared" si="35"/>
+        <v>580</v>
+      </c>
+      <c r="AG142" s="3">
+        <f t="shared" si="35"/>
+        <v>600</v>
       </c>
       <c r="AH142" s="1"/>
       <c r="AI142" s="1"/>
@@ -10021,119 +10055,119 @@
         <v>147</v>
       </c>
       <c r="E143" s="1">
-        <f t="shared" ref="E143:AG143" si="32">E144+E145+E146+E147</f>
+        <f>E144+E145+E146+E147</f>
         <v>7</v>
       </c>
       <c r="F143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="E143:AG143" si="36">F144+F145+F146+F147</f>
         <v>12</v>
       </c>
       <c r="G143" s="1">
-        <f t="shared" si="32"/>
+        <f>G144+G145+G146+G147</f>
         <v>8</v>
       </c>
       <c r="H143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J143" s="1">
-        <f t="shared" si="32"/>
+        <f>J144+J145+J146+J147</f>
         <v>0</v>
       </c>
       <c r="K143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="N143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="P143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Q143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="R143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="S143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="U143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="V143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="X143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Y143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AA143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AB143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="AC143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>35</v>
       </c>
       <c r="AD143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>64</v>
       </c>
       <c r="AE143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="AF143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="AG143" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>9</v>
       </c>
       <c r="AH143" s="1"/>
@@ -10548,119 +10582,119 @@
         <v>496372</v>
       </c>
       <c r="E148" s="3">
-        <f t="shared" ref="E148:AG148" si="33">E149+E150+E151+E152</f>
+        <f t="shared" ref="E148:AG148" si="37">E149+E150+E151+E152</f>
         <v>11689</v>
       </c>
       <c r="F148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>27099</v>
       </c>
       <c r="G148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>26976</v>
       </c>
       <c r="H148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>25708</v>
       </c>
       <c r="I148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>26030</v>
       </c>
       <c r="J148" s="3">
-        <f t="shared" si="33"/>
+        <f>J149+J150+J151+J152</f>
         <v>23850</v>
       </c>
       <c r="K148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>22749</v>
       </c>
       <c r="L148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>22012</v>
       </c>
       <c r="M148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>21151</v>
       </c>
       <c r="N148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19945</v>
       </c>
       <c r="O148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19615</v>
       </c>
       <c r="P148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>18972</v>
       </c>
       <c r="Q148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19270</v>
       </c>
       <c r="R148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19133</v>
       </c>
       <c r="S148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>18986</v>
       </c>
       <c r="T148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>18953</v>
       </c>
       <c r="U148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19184</v>
       </c>
       <c r="V148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19739</v>
       </c>
       <c r="W148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>19439</v>
       </c>
       <c r="X148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>18053</v>
       </c>
       <c r="Y148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>17649</v>
       </c>
       <c r="Z148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>17305</v>
       </c>
       <c r="AA148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>16556</v>
       </c>
       <c r="AB148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>15838</v>
       </c>
       <c r="AC148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>15091</v>
       </c>
       <c r="AD148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>13818</v>
       </c>
       <c r="AE148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>12841</v>
       </c>
       <c r="AF148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>12247</v>
       </c>
       <c r="AG148" s="3">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>11641</v>
       </c>
       <c r="AH148" s="1"/>
@@ -11075,119 +11109,119 @@
         <v>995</v>
       </c>
       <c r="E153" s="1">
-        <f t="shared" ref="E153:AG153" si="34">E155+E154+E156+E157</f>
+        <f t="shared" ref="E153:AG153" si="38">E155+E154+E156+E157</f>
         <v>0</v>
       </c>
       <c r="F153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="H153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>11</v>
       </c>
       <c r="I153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>17</v>
       </c>
       <c r="J153" s="1">
-        <f t="shared" si="34"/>
+        <f>J155+J154+J156+J157</f>
         <v>10</v>
       </c>
       <c r="K153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>12</v>
       </c>
       <c r="L153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>17</v>
       </c>
       <c r="M153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>15</v>
       </c>
       <c r="N153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>22</v>
       </c>
       <c r="O153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>25</v>
       </c>
       <c r="P153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>14</v>
       </c>
       <c r="Q153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>40</v>
       </c>
       <c r="R153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>44</v>
       </c>
       <c r="S153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>37</v>
       </c>
       <c r="T153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>43</v>
       </c>
       <c r="U153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>57</v>
       </c>
       <c r="V153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>55</v>
       </c>
       <c r="W153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>64</v>
       </c>
       <c r="X153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>36</v>
       </c>
       <c r="Y153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>51</v>
       </c>
       <c r="Z153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>39</v>
       </c>
       <c r="AA153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>53</v>
       </c>
       <c r="AB153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>54</v>
       </c>
       <c r="AC153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>68</v>
       </c>
       <c r="AD153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>50</v>
       </c>
       <c r="AE153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>59</v>
       </c>
       <c r="AF153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>54</v>
       </c>
       <c r="AG153" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>71</v>
       </c>
       <c r="AH153" s="1"/>
@@ -11602,119 +11636,119 @@
         <v>480</v>
       </c>
       <c r="E158" s="1">
-        <f t="shared" ref="E158:AG158" si="35">E159+E160+E161+E162</f>
+        <f t="shared" ref="E158:AG158" si="39">E159+E160+E161+E162</f>
         <v>0</v>
       </c>
       <c r="F158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="G158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="H158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>3</v>
       </c>
       <c r="I158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>3</v>
       </c>
       <c r="J158" s="1">
-        <f t="shared" si="35"/>
+        <f>J159+J160+J161+J162</f>
         <v>5</v>
       </c>
       <c r="K158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>3</v>
       </c>
       <c r="L158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
       <c r="M158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="N158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
       <c r="O158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
       <c r="P158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
       <c r="Q158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
       <c r="R158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>11</v>
       </c>
       <c r="S158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>24</v>
       </c>
       <c r="T158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>19</v>
       </c>
       <c r="U158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>26</v>
       </c>
       <c r="V158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>24</v>
       </c>
       <c r="W158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>31</v>
       </c>
       <c r="X158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>36</v>
       </c>
       <c r="Y158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>39</v>
       </c>
       <c r="Z158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>44</v>
       </c>
       <c r="AA158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>27</v>
       </c>
       <c r="AB158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>33</v>
       </c>
       <c r="AC158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>26</v>
       </c>
       <c r="AD158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>21</v>
       </c>
       <c r="AE158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>17</v>
       </c>
       <c r="AF158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>16</v>
       </c>
       <c r="AG158" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>27</v>
       </c>
       <c r="AH158" s="1"/>
@@ -12129,119 +12163,119 @@
         <v>217219</v>
       </c>
       <c r="E163" s="3">
-        <f t="shared" ref="E163:AG163" si="36">E164+E165+E166+E167</f>
+        <f t="shared" ref="E163:AG163" si="40">E164+E165+E166+E167</f>
         <v>6438</v>
       </c>
       <c r="F163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>14253</v>
       </c>
       <c r="G163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>13027</v>
       </c>
       <c r="H163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>12413</v>
       </c>
       <c r="I163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>13334</v>
       </c>
       <c r="J163" s="3">
-        <f t="shared" si="36"/>
+        <f>J164+J165+J166+J167</f>
         <v>13853</v>
       </c>
       <c r="K163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>14119</v>
       </c>
       <c r="L163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>14301</v>
       </c>
       <c r="M163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>13844</v>
       </c>
       <c r="N163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>12377</v>
       </c>
       <c r="O163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>11162</v>
       </c>
       <c r="P163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>10689</v>
       </c>
       <c r="Q163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>10177</v>
       </c>
       <c r="R163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>9349</v>
       </c>
       <c r="S163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>8736</v>
       </c>
       <c r="T163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>8429</v>
       </c>
       <c r="U163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>7209</v>
       </c>
       <c r="V163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>6067</v>
       </c>
       <c r="W163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>5110</v>
       </c>
       <c r="X163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>4172</v>
       </c>
       <c r="Y163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>3071</v>
       </c>
       <c r="Z163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2980</v>
       </c>
       <c r="AA163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2480</v>
       </c>
       <c r="AB163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2598</v>
       </c>
       <c r="AC163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>2170</v>
       </c>
       <c r="AD163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1902</v>
       </c>
       <c r="AE163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1831</v>
       </c>
       <c r="AF163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1758</v>
       </c>
       <c r="AG163" s="3">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1923</v>
       </c>
       <c r="AH163" s="1"/>
@@ -12778,7 +12812,7 @@
     </row>
     <row r="172" spans="1:35">
       <c r="A172" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>9</v>
@@ -12787,94 +12821,124 @@
         <v>3</v>
       </c>
       <c r="E172" s="3">
-        <v>308327</v>
+        <f>SUM(E173,E174,E175,E176)</f>
+        <v>308602</v>
       </c>
       <c r="F172" s="3">
+        <f t="shared" ref="F172:AH172" si="41">SUM(F173,F174,F175,F176)</f>
         <v>8673</v>
       </c>
       <c r="G172" s="3">
+        <f t="shared" si="41"/>
         <v>19617</v>
       </c>
       <c r="H172" s="3">
+        <f t="shared" si="41"/>
         <v>18682</v>
       </c>
       <c r="I172" s="3">
+        <f t="shared" si="41"/>
         <v>17573</v>
       </c>
       <c r="J172" s="3">
+        <f t="shared" si="41"/>
         <v>16518</v>
       </c>
       <c r="K172" s="3">
+        <f t="shared" si="41"/>
         <v>14714</v>
       </c>
       <c r="L172" s="3">
+        <f t="shared" si="41"/>
         <v>14022</v>
       </c>
       <c r="M172" s="3">
+        <f t="shared" si="41"/>
         <v>13418</v>
       </c>
       <c r="N172" s="3">
+        <f t="shared" si="41"/>
         <v>12236</v>
       </c>
       <c r="O172" s="3">
+        <f t="shared" si="41"/>
         <v>11559</v>
       </c>
       <c r="P172" s="3">
-        <v>11152</v>
+        <f t="shared" si="41"/>
+        <v>11153</v>
       </c>
       <c r="Q172" s="3">
-        <v>10850</v>
+        <f t="shared" si="41"/>
+        <v>10851</v>
       </c>
       <c r="R172" s="3">
+        <f t="shared" si="41"/>
         <v>11026</v>
       </c>
       <c r="S172" s="3">
-        <v>10600</v>
+        <f t="shared" si="41"/>
+        <v>10601</v>
       </c>
       <c r="T172" s="3">
-        <v>10430</v>
+        <f t="shared" si="41"/>
+        <v>10432</v>
       </c>
       <c r="U172" s="3">
+        <f t="shared" si="41"/>
         <v>10527</v>
       </c>
       <c r="V172" s="3">
-        <v>10572</v>
+        <f t="shared" si="41"/>
+        <v>10573</v>
       </c>
       <c r="W172" s="3">
-        <v>10600</v>
+        <f t="shared" si="41"/>
+        <v>10605</v>
       </c>
       <c r="X172" s="3">
-        <v>9864</v>
+        <f t="shared" si="41"/>
+        <v>9868</v>
       </c>
       <c r="Y172" s="3">
-        <v>9293</v>
+        <f t="shared" si="41"/>
+        <v>9294</v>
       </c>
       <c r="Z172" s="3">
-        <v>8602</v>
+        <f t="shared" si="41"/>
+        <v>8604</v>
       </c>
       <c r="AA172" s="3">
+        <f t="shared" si="41"/>
         <v>8453</v>
       </c>
       <c r="AB172" s="3">
-        <v>8168</v>
+        <f t="shared" si="41"/>
+        <v>8169</v>
       </c>
       <c r="AC172" s="3">
+        <f t="shared" si="41"/>
         <v>8040</v>
       </c>
       <c r="AD172" s="3">
+        <f t="shared" si="41"/>
         <v>7993</v>
       </c>
       <c r="AE172" s="3">
+        <f t="shared" si="41"/>
         <v>7991</v>
       </c>
       <c r="AF172" s="3">
+        <f t="shared" si="41"/>
         <v>7728</v>
       </c>
       <c r="AG172" s="3">
+        <f t="shared" si="41"/>
         <v>7659</v>
       </c>
       <c r="AH172" s="3">
-        <v>7636</v>
+        <f t="shared" si="41"/>
+        <v>7638</v>
       </c>
     </row>
     <row r="173" spans="1:35">
@@ -12884,94 +12948,124 @@
         <v>4</v>
       </c>
       <c r="E173" s="3">
-        <v>140198</v>
+        <f>SUM(E178,E182,E187,E192,E197)</f>
+        <v>140322</v>
       </c>
       <c r="F173" s="3">
+        <f t="shared" ref="F173:AH173" si="42">SUM(F178,F182,F187,F192,F197)</f>
         <v>4073</v>
       </c>
       <c r="G173" s="3">
+        <f t="shared" si="42"/>
         <v>9173</v>
       </c>
       <c r="H173" s="3">
+        <f t="shared" si="42"/>
         <v>8734</v>
       </c>
       <c r="I173" s="3">
+        <f t="shared" si="42"/>
         <v>8111</v>
       </c>
       <c r="J173" s="3">
+        <f t="shared" si="42"/>
         <v>7612</v>
       </c>
       <c r="K173" s="3">
+        <f t="shared" si="42"/>
         <v>6683</v>
       </c>
       <c r="L173" s="3">
+        <f t="shared" si="42"/>
         <v>6500</v>
       </c>
       <c r="M173" s="3">
+        <f t="shared" si="42"/>
         <v>6096</v>
       </c>
       <c r="N173" s="3">
+        <f t="shared" si="42"/>
         <v>5662</v>
       </c>
       <c r="O173" s="3">
+        <f t="shared" si="42"/>
         <v>5242</v>
       </c>
       <c r="P173" s="3">
+        <f t="shared" si="42"/>
         <v>5121</v>
       </c>
       <c r="Q173" s="3">
+        <f t="shared" si="42"/>
         <v>4892</v>
       </c>
       <c r="R173" s="3">
+        <f t="shared" si="42"/>
         <v>5050</v>
       </c>
       <c r="S173" s="3">
-        <v>4878</v>
+        <f t="shared" si="42"/>
+        <v>4879</v>
       </c>
       <c r="T173" s="3">
+        <f t="shared" si="42"/>
         <v>4722</v>
       </c>
       <c r="U173" s="3">
+        <f t="shared" si="42"/>
         <v>4653</v>
       </c>
       <c r="V173" s="3">
-        <v>4897</v>
+        <f t="shared" si="42"/>
+        <v>4898</v>
       </c>
       <c r="W173" s="3">
-        <v>4772</v>
+        <f t="shared" si="42"/>
+        <v>4774</v>
       </c>
       <c r="X173" s="3">
-        <v>4440</v>
+        <f t="shared" si="42"/>
+        <v>4442</v>
       </c>
       <c r="Y173" s="3">
+        <f t="shared" si="42"/>
         <v>4235</v>
       </c>
       <c r="Z173" s="3">
-        <v>3983</v>
+        <f t="shared" si="42"/>
+        <v>3984</v>
       </c>
       <c r="AA173" s="3">
+        <f t="shared" si="42"/>
         <v>3729</v>
       </c>
       <c r="AB173" s="3">
+        <f t="shared" si="42"/>
         <v>3585</v>
       </c>
       <c r="AC173" s="3">
+        <f t="shared" si="42"/>
         <v>3561</v>
       </c>
       <c r="AD173" s="3">
+        <f t="shared" si="42"/>
         <v>3422</v>
       </c>
       <c r="AE173" s="3">
+        <f t="shared" si="42"/>
         <v>3534</v>
       </c>
       <c r="AF173" s="3">
+        <f t="shared" si="42"/>
         <v>3400</v>
       </c>
       <c r="AG173" s="3">
+        <f t="shared" si="42"/>
         <v>3361</v>
       </c>
       <c r="AH173" s="3">
-        <v>3426</v>
+        <f t="shared" si="42"/>
+        <v>3427</v>
       </c>
     </row>
     <row r="174" spans="1:35">
@@ -12981,94 +13075,124 @@
         <v>5</v>
       </c>
       <c r="E174" s="3">
-        <v>110853</v>
+        <f>SUM(E179,E183,E188,E193,E198)</f>
+        <v>110950</v>
       </c>
       <c r="F174" s="3">
+        <f t="shared" ref="F174:AH174" si="43">SUM(F179,F183,F188,F193,F198)</f>
         <v>2893</v>
       </c>
       <c r="G174" s="3">
+        <f t="shared" si="43"/>
         <v>6631</v>
       </c>
       <c r="H174" s="3">
+        <f t="shared" si="43"/>
         <v>6428</v>
       </c>
       <c r="I174" s="3">
+        <f t="shared" si="43"/>
         <v>6110</v>
       </c>
       <c r="J174" s="3">
+        <f t="shared" si="43"/>
         <v>5742</v>
       </c>
       <c r="K174" s="3">
+        <f t="shared" si="43"/>
         <v>5091</v>
       </c>
       <c r="L174" s="3">
+        <f t="shared" si="43"/>
         <v>4895</v>
       </c>
       <c r="M174" s="3">
+        <f t="shared" si="43"/>
         <v>4834</v>
       </c>
       <c r="N174" s="3">
+        <f t="shared" si="43"/>
         <v>4248</v>
       </c>
       <c r="O174" s="3">
+        <f t="shared" si="43"/>
         <v>4224</v>
       </c>
       <c r="P174" s="3">
-        <v>4026</v>
+        <f t="shared" si="43"/>
+        <v>4027</v>
       </c>
       <c r="Q174" s="3">
-        <v>3915</v>
+        <f t="shared" si="43"/>
+        <v>3916</v>
       </c>
       <c r="R174" s="3">
+        <f t="shared" si="43"/>
         <v>3964</v>
       </c>
       <c r="S174" s="3">
+        <f t="shared" si="43"/>
         <v>3714</v>
       </c>
       <c r="T174" s="3">
-        <v>3810</v>
+        <f t="shared" si="43"/>
+        <v>3812</v>
       </c>
       <c r="U174" s="3">
+        <f t="shared" si="43"/>
         <v>3866</v>
       </c>
       <c r="V174" s="3">
+        <f t="shared" si="43"/>
         <v>3772</v>
       </c>
       <c r="W174" s="3">
-        <v>3847</v>
+        <f t="shared" si="43"/>
+        <v>3849</v>
       </c>
       <c r="X174" s="3">
-        <v>3636</v>
+        <f t="shared" si="43"/>
+        <v>3638</v>
       </c>
       <c r="Y174" s="3">
-        <v>3396</v>
+        <f t="shared" si="43"/>
+        <v>3397</v>
       </c>
       <c r="Z174" s="3">
-        <v>3178</v>
+        <f t="shared" si="43"/>
+        <v>3179</v>
       </c>
       <c r="AA174" s="3">
+        <f t="shared" si="43"/>
         <v>3245</v>
       </c>
       <c r="AB174" s="3">
-        <v>3155</v>
+        <f t="shared" si="43"/>
+        <v>3156</v>
       </c>
       <c r="AC174" s="3">
+        <f t="shared" si="43"/>
         <v>3105</v>
       </c>
       <c r="AD174" s="3">
+        <f t="shared" si="43"/>
         <v>3067</v>
       </c>
       <c r="AE174" s="3">
+        <f t="shared" si="43"/>
         <v>3078</v>
       </c>
       <c r="AF174" s="3">
+        <f t="shared" si="43"/>
         <v>2981</v>
       </c>
       <c r="AG174" s="3">
+        <f t="shared" si="43"/>
         <v>3040</v>
       </c>
       <c r="AH174" s="3">
-        <v>2915</v>
+        <f t="shared" si="43"/>
+        <v>2916</v>
       </c>
     </row>
     <row r="175" spans="1:35">
@@ -13078,93 +13202,123 @@
         <v>6</v>
       </c>
       <c r="E175" s="3">
-        <v>41478</v>
+        <f>SUM(E180,E184,E189,E194,E199)</f>
+        <v>41502</v>
       </c>
       <c r="F175" s="3">
+        <f t="shared" ref="F175:AH175" si="44">SUM(F180,F184,F189,F194,F199)</f>
         <v>1297</v>
       </c>
       <c r="G175" s="3">
+        <f t="shared" si="44"/>
         <v>2892</v>
       </c>
       <c r="H175" s="3">
+        <f t="shared" si="44"/>
         <v>2677</v>
       </c>
       <c r="I175" s="3">
+        <f t="shared" si="44"/>
         <v>2477</v>
       </c>
       <c r="J175" s="3">
+        <f t="shared" si="44"/>
         <v>2278</v>
       </c>
       <c r="K175" s="3">
+        <f t="shared" si="44"/>
         <v>2168</v>
       </c>
       <c r="L175" s="3">
+        <f t="shared" si="44"/>
         <v>1898</v>
       </c>
       <c r="M175" s="3">
+        <f t="shared" si="44"/>
         <v>1860</v>
       </c>
       <c r="N175" s="3">
+        <f t="shared" si="44"/>
         <v>1599</v>
       </c>
       <c r="O175" s="3">
+        <f t="shared" si="44"/>
         <v>1522</v>
       </c>
       <c r="P175" s="3">
+        <f t="shared" si="44"/>
         <v>1423</v>
       </c>
       <c r="Q175" s="3">
+        <f t="shared" si="44"/>
         <v>1430</v>
       </c>
       <c r="R175" s="3">
+        <f t="shared" si="44"/>
         <v>1420</v>
       </c>
       <c r="S175" s="3">
+        <f t="shared" si="44"/>
         <v>1422</v>
       </c>
       <c r="T175" s="3">
+        <f t="shared" si="44"/>
         <v>1347</v>
       </c>
       <c r="U175" s="3">
+        <f t="shared" si="44"/>
         <v>1474</v>
       </c>
       <c r="V175" s="3">
+        <f t="shared" si="44"/>
         <v>1326</v>
       </c>
       <c r="W175" s="3">
-        <v>1407</v>
+        <f t="shared" si="44"/>
+        <v>1408</v>
       </c>
       <c r="X175" s="3">
+        <f t="shared" si="44"/>
         <v>1258</v>
       </c>
       <c r="Y175" s="3">
+        <f t="shared" si="44"/>
         <v>1225</v>
       </c>
       <c r="Z175" s="3">
+        <f t="shared" si="44"/>
         <v>1015</v>
       </c>
       <c r="AA175" s="3">
+        <f t="shared" si="44"/>
         <v>1025</v>
       </c>
-      <c r="AB175" s="1">
+      <c r="AB175" s="3">
+        <f t="shared" si="44"/>
         <v>981</v>
       </c>
-      <c r="AC175" s="1">
+      <c r="AC175" s="3">
+        <f t="shared" si="44"/>
         <v>957</v>
       </c>
       <c r="AD175" s="3">
+        <f t="shared" si="44"/>
         <v>1037</v>
       </c>
-      <c r="AE175" s="1">
+      <c r="AE175" s="3">
+        <f t="shared" si="44"/>
         <v>998</v>
       </c>
-      <c r="AF175" s="1">
+      <c r="AF175" s="3">
+        <f t="shared" si="44"/>
         <v>958</v>
       </c>
-      <c r="AG175" s="1">
+      <c r="AG175" s="3">
+        <f t="shared" si="44"/>
         <v>836</v>
       </c>
-      <c r="AH175" s="1">
+      <c r="AH175" s="3">
+        <f t="shared" si="44"/>
         <v>896</v>
       </c>
     </row>
@@ -13175,93 +13329,123 @@
         <v>7</v>
       </c>
       <c r="E176" s="3">
-        <v>15812</v>
-      </c>
-      <c r="F176" s="1">
+        <f>SUM(E185,E190,E195,E200)</f>
+        <v>15828</v>
+      </c>
+      <c r="F176" s="3">
+        <f t="shared" ref="F176:AH176" si="45">SUM(F185,F190,F195,F200)</f>
         <v>410</v>
       </c>
-      <c r="G176" s="1">
+      <c r="G176" s="3">
+        <f t="shared" si="45"/>
         <v>921</v>
       </c>
-      <c r="H176" s="1">
+      <c r="H176" s="3">
+        <f t="shared" si="45"/>
         <v>843</v>
       </c>
-      <c r="I176" s="1">
+      <c r="I176" s="3">
+        <f t="shared" si="45"/>
         <v>875</v>
       </c>
-      <c r="J176" s="1">
+      <c r="J176" s="3">
+        <f t="shared" si="45"/>
         <v>886</v>
       </c>
-      <c r="K176" s="1">
+      <c r="K176" s="3">
+        <f t="shared" si="45"/>
         <v>772</v>
       </c>
-      <c r="L176" s="1">
+      <c r="L176" s="3">
+        <f t="shared" si="45"/>
         <v>729</v>
       </c>
-      <c r="M176" s="1">
+      <c r="M176" s="3">
+        <f t="shared" si="45"/>
         <v>628</v>
       </c>
-      <c r="N176" s="1">
+      <c r="N176" s="3">
+        <f t="shared" si="45"/>
         <v>727</v>
       </c>
-      <c r="O176" s="1">
+      <c r="O176" s="3">
+        <f t="shared" si="45"/>
         <v>571</v>
       </c>
-      <c r="P176" s="1">
+      <c r="P176" s="3">
+        <f t="shared" si="45"/>
         <v>582</v>
       </c>
-      <c r="Q176" s="1">
+      <c r="Q176" s="3">
+        <f t="shared" si="45"/>
         <v>613</v>
       </c>
-      <c r="R176" s="1">
+      <c r="R176" s="3">
+        <f t="shared" si="45"/>
         <v>592</v>
       </c>
-      <c r="S176" s="1">
+      <c r="S176" s="3">
+        <f t="shared" si="45"/>
         <v>586</v>
       </c>
-      <c r="T176" s="1">
+      <c r="T176" s="3">
+        <f t="shared" si="45"/>
         <v>551</v>
       </c>
-      <c r="U176" s="1">
+      <c r="U176" s="3">
+        <f t="shared" si="45"/>
         <v>534</v>
       </c>
-      <c r="V176" s="1">
+      <c r="V176" s="3">
+        <f t="shared" si="45"/>
         <v>577</v>
       </c>
-      <c r="W176" s="1">
+      <c r="W176" s="3">
+        <f t="shared" si="45"/>
         <v>574</v>
       </c>
-      <c r="X176" s="1">
+      <c r="X176" s="3">
+        <f t="shared" si="45"/>
         <v>530</v>
       </c>
-      <c r="Y176" s="1">
+      <c r="Y176" s="3">
+        <f t="shared" si="45"/>
         <v>437</v>
       </c>
-      <c r="Z176" s="1">
+      <c r="Z176" s="3">
+        <f t="shared" si="45"/>
         <v>426</v>
       </c>
-      <c r="AA176" s="1">
+      <c r="AA176" s="3">
+        <f t="shared" si="45"/>
         <v>454</v>
       </c>
-      <c r="AB176" s="1">
+      <c r="AB176" s="3">
+        <f t="shared" si="45"/>
         <v>447</v>
       </c>
-      <c r="AC176" s="1">
+      <c r="AC176" s="3">
+        <f t="shared" si="45"/>
         <v>417</v>
       </c>
-      <c r="AD176" s="1">
+      <c r="AD176" s="3">
+        <f t="shared" si="45"/>
         <v>467</v>
       </c>
-      <c r="AE176" s="1">
+      <c r="AE176" s="3">
+        <f t="shared" si="45"/>
         <v>381</v>
       </c>
-      <c r="AF176" s="1">
+      <c r="AF176" s="3">
+        <f t="shared" si="45"/>
         <v>389</v>
       </c>
-      <c r="AG176" s="1">
+      <c r="AG176" s="3">
+        <f t="shared" si="45"/>
         <v>422</v>
       </c>
-      <c r="AH176" s="1">
+      <c r="AH176" s="3">
+        <f t="shared" si="45"/>
         <v>399</v>
       </c>
     </row>
@@ -15620,7 +15804,7 @@
     </row>
     <row r="205" spans="1:34">
       <c r="A205" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B205" s="19"/>
       <c r="C205" s="1"/>
@@ -15718,7 +15902,7 @@
     </row>
     <row r="206" spans="1:34">
       <c r="A206" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>9</v>
@@ -15729,123 +15913,123 @@
       <c r="D206" s="1"/>
       <c r="E206" s="3">
         <f>E210+E209+E208+E207</f>
-        <v>112656</v>
+        <v>114364</v>
       </c>
       <c r="F206" s="3">
-        <f t="shared" ref="F206:AH206" si="37">F210+F209+F208+F207</f>
-        <v>1397</v>
+        <f t="shared" ref="F206:AH206" si="46">F210+F209+F208+F207</f>
+        <v>1415</v>
       </c>
       <c r="G206" s="3">
-        <f t="shared" si="37"/>
-        <v>4303</v>
+        <f t="shared" si="46"/>
+        <v>4379</v>
       </c>
       <c r="H206" s="3">
-        <f t="shared" si="37"/>
-        <v>4972</v>
+        <f t="shared" si="46"/>
+        <v>5086</v>
       </c>
       <c r="I206" s="3">
-        <f t="shared" si="37"/>
-        <v>4881</v>
+        <f t="shared" si="46"/>
+        <v>4974</v>
       </c>
       <c r="J206" s="3">
-        <f t="shared" si="37"/>
-        <v>3870</v>
+        <f t="shared" si="46"/>
+        <v>3953</v>
       </c>
       <c r="K206" s="3">
-        <f t="shared" si="37"/>
-        <v>4102</v>
+        <f t="shared" si="46"/>
+        <v>4163</v>
       </c>
       <c r="L206" s="3">
-        <f t="shared" si="37"/>
-        <v>4297</v>
+        <f t="shared" si="46"/>
+        <v>4377</v>
       </c>
       <c r="M206" s="3">
-        <f t="shared" si="37"/>
-        <v>4691</v>
+        <f t="shared" si="46"/>
+        <v>4782</v>
       </c>
       <c r="N206" s="3">
-        <f t="shared" si="37"/>
-        <v>4796</v>
+        <f t="shared" si="46"/>
+        <v>4863</v>
       </c>
       <c r="O206" s="3">
-        <f t="shared" si="37"/>
-        <v>4752</v>
+        <f t="shared" si="46"/>
+        <v>4834</v>
       </c>
       <c r="P206" s="3">
-        <f t="shared" si="37"/>
-        <v>4607</v>
+        <f t="shared" si="46"/>
+        <v>4676</v>
       </c>
       <c r="Q206" s="3">
-        <f t="shared" si="37"/>
-        <v>4619</v>
+        <f t="shared" si="46"/>
+        <v>4701</v>
       </c>
       <c r="R206" s="3">
-        <f t="shared" si="37"/>
-        <v>4783</v>
+        <f t="shared" si="46"/>
+        <v>4866</v>
       </c>
       <c r="S206" s="3">
-        <f t="shared" si="37"/>
-        <v>4678</v>
+        <f t="shared" si="46"/>
+        <v>4750</v>
       </c>
       <c r="T206" s="3">
-        <f t="shared" si="37"/>
-        <v>4688</v>
+        <f t="shared" si="46"/>
+        <v>4747</v>
       </c>
       <c r="U206" s="3">
-        <f t="shared" si="37"/>
-        <v>4653</v>
+        <f t="shared" si="46"/>
+        <v>4729</v>
       </c>
       <c r="V206" s="3">
-        <f t="shared" si="37"/>
-        <v>4543</v>
+        <f t="shared" si="46"/>
+        <v>4608</v>
       </c>
       <c r="W206" s="3">
-        <f t="shared" si="37"/>
-        <v>4517</v>
+        <f t="shared" si="46"/>
+        <v>4575</v>
       </c>
       <c r="X206" s="3">
-        <f t="shared" si="37"/>
-        <v>4175</v>
+        <f t="shared" si="46"/>
+        <v>4228</v>
       </c>
       <c r="Y206" s="3">
-        <f t="shared" si="37"/>
-        <v>4084</v>
+        <f t="shared" si="46"/>
+        <v>4132</v>
       </c>
       <c r="Z206" s="3">
-        <f t="shared" si="37"/>
-        <v>3881</v>
+        <f t="shared" si="46"/>
+        <v>3918</v>
       </c>
       <c r="AA206" s="3">
-        <f t="shared" si="37"/>
-        <v>3795</v>
+        <f t="shared" si="46"/>
+        <v>3825</v>
       </c>
       <c r="AB206" s="3">
-        <f t="shared" si="37"/>
-        <v>3433</v>
+        <f t="shared" si="46"/>
+        <v>3474</v>
       </c>
       <c r="AC206" s="3">
-        <f t="shared" si="37"/>
-        <v>3187</v>
+        <f t="shared" si="46"/>
+        <v>3214</v>
       </c>
       <c r="AD206" s="3">
-        <f t="shared" si="37"/>
-        <v>3310</v>
+        <f t="shared" si="46"/>
+        <v>3330</v>
       </c>
       <c r="AE206" s="3">
-        <f t="shared" si="37"/>
-        <v>2432</v>
+        <f t="shared" si="46"/>
+        <v>2449</v>
       </c>
       <c r="AF206" s="3">
-        <f t="shared" si="37"/>
-        <v>2071</v>
+        <f t="shared" si="46"/>
+        <v>2084</v>
       </c>
       <c r="AG206" s="3">
-        <f t="shared" si="37"/>
-        <v>1846</v>
+        <f t="shared" si="46"/>
+        <v>1864</v>
       </c>
       <c r="AH206" s="3">
-        <f t="shared" si="37"/>
-        <v>1531</v>
+        <f t="shared" si="46"/>
+        <v>1540</v>
       </c>
     </row>
     <row r="207" spans="1:34">
@@ -15856,94 +16040,124 @@
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="3">
-        <v>58818</v>
-      </c>
-      <c r="F207" s="1">
-        <v>728</v>
+        <f>SUM(E212,E216,E221,E226,E231)</f>
+        <v>59781</v>
+      </c>
+      <c r="F207" s="3">
+        <f t="shared" ref="F207:AH207" si="47">SUM(F212,F216,F221,F226,F231)</f>
+        <v>738</v>
       </c>
       <c r="G207" s="3">
-        <v>2303</v>
+        <f t="shared" si="47"/>
+        <v>2344</v>
       </c>
       <c r="H207" s="3">
-        <v>2644</v>
+        <f t="shared" si="47"/>
+        <v>2721</v>
       </c>
       <c r="I207" s="3">
-        <v>2644</v>
+        <f t="shared" si="47"/>
+        <v>2699</v>
       </c>
       <c r="J207" s="3">
-        <v>2102</v>
+        <f t="shared" si="47"/>
+        <v>2137</v>
       </c>
       <c r="K207" s="3">
-        <v>2207</v>
+        <f t="shared" si="47"/>
+        <v>2246</v>
       </c>
       <c r="L207" s="3">
-        <v>2230</v>
+        <f t="shared" si="47"/>
+        <v>2278</v>
       </c>
       <c r="M207" s="3">
-        <v>2444</v>
+        <f t="shared" si="47"/>
+        <v>2497</v>
       </c>
       <c r="N207" s="3">
-        <v>2484</v>
+        <f t="shared" si="47"/>
+        <v>2521</v>
       </c>
       <c r="O207" s="3">
-        <v>2412</v>
+        <f t="shared" si="47"/>
+        <v>2452</v>
       </c>
       <c r="P207" s="3">
-        <v>2383</v>
+        <f t="shared" si="47"/>
+        <v>2423</v>
       </c>
       <c r="Q207" s="3">
-        <v>2414</v>
+        <f t="shared" si="47"/>
+        <v>2462</v>
       </c>
       <c r="R207" s="3">
-        <v>2453</v>
+        <f t="shared" si="47"/>
+        <v>2508</v>
       </c>
       <c r="S207" s="3">
-        <v>2427</v>
+        <f t="shared" si="47"/>
+        <v>2469</v>
       </c>
       <c r="T207" s="3">
-        <v>2458</v>
+        <f t="shared" si="47"/>
+        <v>2493</v>
       </c>
       <c r="U207" s="3">
-        <v>2461</v>
+        <f t="shared" si="47"/>
+        <v>2506</v>
       </c>
       <c r="V207" s="3">
-        <v>2333</v>
+        <f t="shared" si="47"/>
+        <v>2371</v>
       </c>
       <c r="W207" s="3">
-        <v>2305</v>
+        <f t="shared" si="47"/>
+        <v>2334</v>
       </c>
       <c r="X207" s="3">
-        <v>2207</v>
+        <f t="shared" si="47"/>
+        <v>2228</v>
       </c>
       <c r="Y207" s="3">
-        <v>2101</v>
+        <f t="shared" si="47"/>
+        <v>2130</v>
       </c>
       <c r="Z207" s="3">
-        <v>1965</v>
+        <f t="shared" si="47"/>
+        <v>1982</v>
       </c>
       <c r="AA207" s="3">
-        <v>2004</v>
+        <f t="shared" si="47"/>
+        <v>2019</v>
       </c>
       <c r="AB207" s="3">
-        <v>1767</v>
+        <f t="shared" si="47"/>
+        <v>1788</v>
       </c>
       <c r="AC207" s="3">
-        <v>1671</v>
+        <f t="shared" si="47"/>
+        <v>1687</v>
       </c>
       <c r="AD207" s="3">
-        <v>1689</v>
+        <f t="shared" si="47"/>
+        <v>1703</v>
       </c>
       <c r="AE207" s="3">
-        <v>1298</v>
+        <f t="shared" si="47"/>
+        <v>1304</v>
       </c>
       <c r="AF207" s="3">
-        <v>1079</v>
-      </c>
-      <c r="AG207" s="1">
-        <v>934</v>
-      </c>
-      <c r="AH207" s="1">
-        <v>798</v>
+        <f t="shared" si="47"/>
+        <v>1084</v>
+      </c>
+      <c r="AG207" s="3">
+        <f t="shared" si="47"/>
+        <v>944</v>
+      </c>
+      <c r="AH207" s="3">
+        <f t="shared" si="47"/>
+        <v>801</v>
       </c>
     </row>
     <row r="208" spans="1:34">
@@ -15954,94 +16168,124 @@
       </c>
       <c r="D208" s="1"/>
       <c r="E208" s="3">
-        <v>32628</v>
-      </c>
-      <c r="F208" s="1">
-        <v>420</v>
+        <f>SUM(E213,E217,E222,E227,E232)</f>
+        <v>33011</v>
+      </c>
+      <c r="F208" s="3">
+        <f t="shared" ref="F208:AH208" si="48">SUM(F213,F217,F222,F227,F232)</f>
+        <v>425</v>
       </c>
       <c r="G208" s="3">
-        <v>1196</v>
+        <f t="shared" si="48"/>
+        <v>1215</v>
       </c>
       <c r="H208" s="3">
-        <v>1413</v>
+        <f t="shared" si="48"/>
+        <v>1431</v>
       </c>
       <c r="I208" s="3">
-        <v>1390</v>
+        <f t="shared" si="48"/>
+        <v>1414</v>
       </c>
       <c r="J208" s="3">
-        <v>1042</v>
+        <f t="shared" si="48"/>
+        <v>1064</v>
       </c>
       <c r="K208" s="3">
-        <v>1144</v>
+        <f t="shared" si="48"/>
+        <v>1156</v>
       </c>
       <c r="L208" s="3">
-        <v>1259</v>
+        <f t="shared" si="48"/>
+        <v>1273</v>
       </c>
       <c r="M208" s="3">
+        <f t="shared" si="48"/>
+        <v>1395</v>
+      </c>
+      <c r="N208" s="3">
+        <f t="shared" si="48"/>
+        <v>1429</v>
+      </c>
+      <c r="O208" s="3">
+        <f t="shared" si="48"/>
+        <v>1447</v>
+      </c>
+      <c r="P208" s="3">
+        <f t="shared" si="48"/>
+        <v>1393</v>
+      </c>
+      <c r="Q208" s="3">
+        <f t="shared" si="48"/>
+        <v>1386</v>
+      </c>
+      <c r="R208" s="3">
+        <f t="shared" si="48"/>
+        <v>1433</v>
+      </c>
+      <c r="S208" s="3">
+        <f t="shared" si="48"/>
+        <v>1362</v>
+      </c>
+      <c r="T208" s="3">
+        <f t="shared" si="48"/>
+        <v>1375</v>
+      </c>
+      <c r="U208" s="3">
+        <f t="shared" si="48"/>
+        <v>1343</v>
+      </c>
+      <c r="V208" s="3">
+        <f t="shared" si="48"/>
+        <v>1361</v>
+      </c>
+      <c r="W208" s="3">
+        <f t="shared" si="48"/>
         <v>1374</v>
       </c>
-      <c r="N208" s="3">
-        <v>1415</v>
-      </c>
-      <c r="O208" s="3">
-        <v>1427</v>
-      </c>
-      <c r="P208" s="3">
-        <v>1380</v>
-      </c>
-      <c r="Q208" s="3">
-        <v>1367</v>
-      </c>
-      <c r="R208" s="3">
-        <v>1418</v>
-      </c>
-      <c r="S208" s="3">
-        <v>1345</v>
-      </c>
-      <c r="T208" s="3">
-        <v>1364</v>
-      </c>
-      <c r="U208" s="3">
-        <v>1333</v>
-      </c>
-      <c r="V208" s="3">
-        <v>1347</v>
-      </c>
-      <c r="W208" s="3">
-        <v>1356</v>
-      </c>
       <c r="X208" s="3">
-        <v>1150</v>
+        <f t="shared" si="48"/>
+        <v>1169</v>
       </c>
       <c r="Y208" s="3">
-        <v>1169</v>
+        <f t="shared" si="48"/>
+        <v>1180</v>
       </c>
       <c r="Z208" s="3">
-        <v>1167</v>
+        <f t="shared" si="48"/>
+        <v>1178</v>
       </c>
       <c r="AA208" s="3">
-        <v>1067</v>
-      </c>
-      <c r="AB208" s="1">
-        <v>997</v>
-      </c>
-      <c r="AC208" s="1">
-        <v>936</v>
-      </c>
-      <c r="AD208" s="1">
-        <v>944</v>
-      </c>
-      <c r="AE208" s="1">
-        <v>665</v>
-      </c>
-      <c r="AF208" s="1">
-        <v>593</v>
-      </c>
-      <c r="AG208" s="1">
-        <v>580</v>
-      </c>
-      <c r="AH208" s="1">
-        <v>430</v>
+        <f t="shared" si="48"/>
+        <v>1072</v>
+      </c>
+      <c r="AB208" s="3">
+        <f t="shared" si="48"/>
+        <v>1008</v>
+      </c>
+      <c r="AC208" s="3">
+        <f t="shared" si="48"/>
+        <v>941</v>
+      </c>
+      <c r="AD208" s="3">
+        <f t="shared" si="48"/>
+        <v>948</v>
+      </c>
+      <c r="AE208" s="3">
+        <f t="shared" si="48"/>
+        <v>668</v>
+      </c>
+      <c r="AF208" s="3">
+        <f t="shared" si="48"/>
+        <v>598</v>
+      </c>
+      <c r="AG208" s="3">
+        <f t="shared" si="48"/>
+        <v>585</v>
+      </c>
+      <c r="AH208" s="3">
+        <f t="shared" si="48"/>
+        <v>432</v>
       </c>
     </row>
     <row r="209" spans="1:34">
@@ -16052,94 +16296,124 @@
       </c>
       <c r="D209" s="1"/>
       <c r="E209" s="3">
-        <v>18074</v>
-      </c>
-      <c r="F209" s="1">
-        <v>217</v>
-      </c>
-      <c r="G209" s="1">
-        <v>719</v>
-      </c>
-      <c r="H209" s="1">
-        <v>809</v>
-      </c>
-      <c r="I209" s="1">
-        <v>722</v>
-      </c>
-      <c r="J209" s="1">
-        <v>630</v>
-      </c>
-      <c r="K209" s="1">
-        <v>649</v>
-      </c>
-      <c r="L209" s="1">
-        <v>710</v>
-      </c>
-      <c r="M209" s="1">
+        <f>SUM(E214,E218,E223,E228,E233)</f>
+        <v>18405</v>
+      </c>
+      <c r="F209" s="3">
+        <f t="shared" ref="F209:AH209" si="49">SUM(F214,F218,F223,F228,F233)</f>
+        <v>220</v>
+      </c>
+      <c r="G209" s="3">
+        <f t="shared" si="49"/>
+        <v>733</v>
+      </c>
+      <c r="H209" s="3">
+        <f t="shared" si="49"/>
+        <v>827</v>
+      </c>
+      <c r="I209" s="3">
+        <f t="shared" si="49"/>
+        <v>735</v>
+      </c>
+      <c r="J209" s="3">
+        <f t="shared" si="49"/>
+        <v>652</v>
+      </c>
+      <c r="K209" s="3">
+        <f t="shared" si="49"/>
+        <v>659</v>
+      </c>
+      <c r="L209" s="3">
+        <f t="shared" si="49"/>
+        <v>727</v>
+      </c>
+      <c r="M209" s="3">
+        <f t="shared" si="49"/>
+        <v>750</v>
+      </c>
+      <c r="N209" s="3">
+        <f t="shared" si="49"/>
+        <v>777</v>
+      </c>
+      <c r="O209" s="3">
+        <f t="shared" si="49"/>
+        <v>789</v>
+      </c>
+      <c r="P209" s="3">
+        <f t="shared" si="49"/>
+        <v>727</v>
+      </c>
+      <c r="Q209" s="3">
+        <f t="shared" si="49"/>
+        <v>727</v>
+      </c>
+      <c r="R209" s="3">
+        <f t="shared" si="49"/>
+        <v>782</v>
+      </c>
+      <c r="S209" s="3">
+        <f t="shared" si="49"/>
+        <v>749</v>
+      </c>
+      <c r="T209" s="3">
+        <f t="shared" si="49"/>
+        <v>729</v>
+      </c>
+      <c r="U209" s="3">
+        <f t="shared" si="49"/>
         <v>734</v>
       </c>
-      <c r="N209" s="1">
-        <v>762</v>
-      </c>
-      <c r="O209" s="1">
-        <v>768</v>
-      </c>
-      <c r="P209" s="1">
-        <v>713</v>
-      </c>
-      <c r="Q209" s="1">
-        <v>714</v>
-      </c>
-      <c r="R209" s="1">
-        <v>769</v>
-      </c>
-      <c r="S209" s="1">
-        <v>737</v>
-      </c>
-      <c r="T209" s="1">
-        <v>717</v>
-      </c>
-      <c r="U209" s="1">
-        <v>715</v>
-      </c>
-      <c r="V209" s="1">
-        <v>753</v>
-      </c>
-      <c r="W209" s="1">
-        <v>710</v>
-      </c>
-      <c r="X209" s="1">
-        <v>710</v>
-      </c>
-      <c r="Y209" s="1">
-        <v>673</v>
-      </c>
-      <c r="Z209" s="1">
-        <v>638</v>
-      </c>
-      <c r="AA209" s="1">
-        <v>621</v>
-      </c>
-      <c r="AB209" s="1">
-        <v>576</v>
-      </c>
-      <c r="AC209" s="1">
-        <v>498</v>
-      </c>
-      <c r="AD209" s="1">
-        <v>569</v>
-      </c>
-      <c r="AE209" s="1">
-        <v>401</v>
-      </c>
-      <c r="AF209" s="1">
-        <v>341</v>
-      </c>
-      <c r="AG209" s="1">
-        <v>286</v>
-      </c>
-      <c r="AH209" s="1">
-        <v>258</v>
+      <c r="V209" s="3">
+        <f t="shared" si="49"/>
+        <v>764</v>
+      </c>
+      <c r="W209" s="3">
+        <f t="shared" si="49"/>
+        <v>720</v>
+      </c>
+      <c r="X209" s="3">
+        <f t="shared" si="49"/>
+        <v>723</v>
+      </c>
+      <c r="Y209" s="3">
+        <f t="shared" si="49"/>
+        <v>679</v>
+      </c>
+      <c r="Z209" s="3">
+        <f t="shared" si="49"/>
+        <v>647</v>
+      </c>
+      <c r="AA209" s="3">
+        <f t="shared" si="49"/>
+        <v>631</v>
+      </c>
+      <c r="AB209" s="3">
+        <f t="shared" si="49"/>
+        <v>585</v>
+      </c>
+      <c r="AC209" s="3">
+        <f t="shared" si="49"/>
+        <v>503</v>
+      </c>
+      <c r="AD209" s="3">
+        <f t="shared" si="49"/>
+        <v>570</v>
+      </c>
+      <c r="AE209" s="3">
+        <f t="shared" si="49"/>
+        <v>408</v>
+      </c>
+      <c r="AF209" s="3">
+        <f t="shared" si="49"/>
+        <v>343</v>
+      </c>
+      <c r="AG209" s="3">
+        <f t="shared" si="49"/>
+        <v>288</v>
+      </c>
+      <c r="AH209" s="3">
+        <f t="shared" si="49"/>
+        <v>261</v>
       </c>
     </row>
     <row r="210" spans="1:34">
@@ -16150,94 +16424,124 @@
       </c>
       <c r="D210" s="1"/>
       <c r="E210" s="3">
-        <v>3136</v>
-      </c>
-      <c r="F210" s="1">
+        <f>SUM(E219,E224,E229,E234)</f>
+        <v>3167</v>
+      </c>
+      <c r="F210" s="3">
+        <f t="shared" ref="F210:AH210" si="50">SUM(F219,F224,F229,F234)</f>
         <v>32</v>
       </c>
-      <c r="G210" s="1">
-        <v>85</v>
-      </c>
-      <c r="H210" s="1">
-        <v>106</v>
-      </c>
-      <c r="I210" s="1">
-        <v>125</v>
-      </c>
-      <c r="J210" s="1">
-        <v>96</v>
-      </c>
-      <c r="K210" s="1">
+      <c r="G210" s="3">
+        <f t="shared" si="50"/>
+        <v>87</v>
+      </c>
+      <c r="H210" s="3">
+        <f t="shared" si="50"/>
+        <v>107</v>
+      </c>
+      <c r="I210" s="3">
+        <f t="shared" si="50"/>
+        <v>126</v>
+      </c>
+      <c r="J210" s="3">
+        <f t="shared" si="50"/>
+        <v>100</v>
+      </c>
+      <c r="K210" s="3">
+        <f t="shared" si="50"/>
         <v>102</v>
       </c>
-      <c r="L210" s="1">
-        <v>98</v>
-      </c>
-      <c r="M210" s="1">
-        <v>139</v>
-      </c>
-      <c r="N210" s="1">
-        <v>135</v>
-      </c>
-      <c r="O210" s="1">
-        <v>145</v>
-      </c>
-      <c r="P210" s="1">
-        <v>131</v>
-      </c>
-      <c r="Q210" s="1">
-        <v>124</v>
-      </c>
-      <c r="R210" s="1">
+      <c r="L210" s="3">
+        <f t="shared" si="50"/>
+        <v>99</v>
+      </c>
+      <c r="M210" s="3">
+        <f t="shared" si="50"/>
+        <v>140</v>
+      </c>
+      <c r="N210" s="3">
+        <f t="shared" si="50"/>
+        <v>136</v>
+      </c>
+      <c r="O210" s="3">
+        <f t="shared" si="50"/>
+        <v>146</v>
+      </c>
+      <c r="P210" s="3">
+        <f t="shared" si="50"/>
+        <v>133</v>
+      </c>
+      <c r="Q210" s="3">
+        <f t="shared" si="50"/>
+        <v>126</v>
+      </c>
+      <c r="R210" s="3">
+        <f t="shared" si="50"/>
         <v>143</v>
       </c>
-      <c r="S210" s="1">
-        <v>169</v>
-      </c>
-      <c r="T210" s="1">
-        <v>149</v>
-      </c>
-      <c r="U210" s="1">
-        <v>144</v>
-      </c>
-      <c r="V210" s="1">
-        <v>110</v>
-      </c>
-      <c r="W210" s="1">
+      <c r="S210" s="3">
+        <f t="shared" si="50"/>
+        <v>170</v>
+      </c>
+      <c r="T210" s="3">
+        <f t="shared" si="50"/>
+        <v>150</v>
+      </c>
+      <c r="U210" s="3">
+        <f t="shared" si="50"/>
         <v>146</v>
       </c>
-      <c r="X210" s="1">
+      <c r="V210" s="3">
+        <f t="shared" si="50"/>
+        <v>112</v>
+      </c>
+      <c r="W210" s="3">
+        <f t="shared" si="50"/>
+        <v>147</v>
+      </c>
+      <c r="X210" s="3">
+        <f t="shared" si="50"/>
         <v>108</v>
       </c>
-      <c r="Y210" s="1">
-        <v>141</v>
-      </c>
-      <c r="Z210" s="1">
+      <c r="Y210" s="3">
+        <f t="shared" si="50"/>
+        <v>143</v>
+      </c>
+      <c r="Z210" s="3">
+        <f t="shared" si="50"/>
         <v>111</v>
       </c>
-      <c r="AA210" s="1">
+      <c r="AA210" s="3">
+        <f t="shared" si="50"/>
         <v>103</v>
       </c>
-      <c r="AB210" s="1">
+      <c r="AB210" s="3">
+        <f t="shared" si="50"/>
         <v>93</v>
       </c>
-      <c r="AC210" s="1">
-        <v>82</v>
-      </c>
-      <c r="AD210" s="1">
-        <v>108</v>
-      </c>
-      <c r="AE210" s="1">
-        <v>68</v>
-      </c>
-      <c r="AF210" s="1">
-        <v>58</v>
-      </c>
-      <c r="AG210" s="1">
+      <c r="AC210" s="3">
+        <f t="shared" si="50"/>
+        <v>83</v>
+      </c>
+      <c r="AD210" s="3">
+        <f t="shared" si="50"/>
+        <v>109</v>
+      </c>
+      <c r="AE210" s="3">
+        <f t="shared" si="50"/>
+        <v>69</v>
+      </c>
+      <c r="AF210" s="3">
+        <f t="shared" si="50"/>
+        <v>59</v>
+      </c>
+      <c r="AG210" s="3">
+        <f t="shared" si="50"/>
+        <v>47</v>
+      </c>
+      <c r="AH210" s="3">
+        <f t="shared" si="50"/>
         <v>46</v>
-      </c>
-      <c r="AH210" s="1">
-        <v>45</v>
       </c>
     </row>
     <row r="211" spans="1:34">
@@ -16254,119 +16558,119 @@
         <v>10</v>
       </c>
       <c r="F211" s="1">
-        <f t="shared" ref="F211:AH211" si="38">F214+F213+F212</f>
+        <f t="shared" ref="F211:AH211" si="51">F214+F213+F212</f>
         <v>1</v>
       </c>
       <c r="G211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
       <c r="H211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="I211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="J211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="K211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="L211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="M211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="N211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="O211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="P211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="Q211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="R211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="S211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="T211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="U211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="V211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="W211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="X211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="Y211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="Z211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AA211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AB211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AC211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AD211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
       <c r="AE211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>5</v>
       </c>
       <c r="AF211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
       <c r="AG211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="AH211" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
     </row>
@@ -16678,119 +16982,119 @@
         <v>54566</v>
       </c>
       <c r="F215" s="3">
-        <f t="shared" ref="F215:AH215" si="39">F219+F218+F217+F216</f>
+        <f t="shared" ref="F215:AH215" si="52">F219+F218+F217+F216</f>
         <v>423</v>
       </c>
       <c r="G215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1388</v>
       </c>
       <c r="H215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1883</v>
       </c>
       <c r="I215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1907</v>
       </c>
       <c r="J215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1546</v>
       </c>
       <c r="K215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1590</v>
       </c>
       <c r="L215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1586</v>
       </c>
       <c r="M215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1734</v>
       </c>
       <c r="N215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1767</v>
       </c>
       <c r="O215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1862</v>
       </c>
       <c r="P215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1783</v>
       </c>
       <c r="Q215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1718</v>
       </c>
       <c r="R215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1848</v>
       </c>
       <c r="S215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1928</v>
       </c>
       <c r="T215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1955</v>
       </c>
       <c r="U215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2079</v>
       </c>
       <c r="V215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2189</v>
       </c>
       <c r="W215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2350</v>
       </c>
       <c r="X215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2302</v>
       </c>
       <c r="Y215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2403</v>
       </c>
       <c r="Z215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2659</v>
       </c>
       <c r="AA215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2774</v>
       </c>
       <c r="AB215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2548</v>
       </c>
       <c r="AC215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2387</v>
       </c>
       <c r="AD215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>2443</v>
       </c>
       <c r="AE215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1763</v>
       </c>
       <c r="AF215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1514</v>
       </c>
       <c r="AG215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1311</v>
       </c>
       <c r="AH215" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="52"/>
         <v>1044</v>
       </c>
     </row>
@@ -17200,119 +17504,119 @@
         <v>135</v>
       </c>
       <c r="F220" s="1">
-        <f t="shared" ref="F220:AH220" si="40">F224+F223+F222+F221</f>
+        <f t="shared" ref="F220:AH220" si="53">F224+F223+F222+F221</f>
         <v>0</v>
       </c>
       <c r="G220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="H220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="I220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="J220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="K220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="L220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>2</v>
       </c>
       <c r="M220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="N220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="O220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>1</v>
       </c>
       <c r="P220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="Q220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>3</v>
       </c>
       <c r="R220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>8</v>
       </c>
       <c r="S220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>10</v>
       </c>
       <c r="T220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>7</v>
       </c>
       <c r="U220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>5</v>
       </c>
       <c r="V220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>10</v>
       </c>
       <c r="W220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>15</v>
       </c>
       <c r="X220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>12</v>
       </c>
       <c r="Y220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>6</v>
       </c>
       <c r="Z220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>7</v>
       </c>
       <c r="AA220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>10</v>
       </c>
       <c r="AB220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>8</v>
       </c>
       <c r="AC220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>3</v>
       </c>
       <c r="AD220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>9</v>
       </c>
       <c r="AE220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>5</v>
       </c>
       <c r="AF220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>3</v>
       </c>
       <c r="AG220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>3</v>
       </c>
       <c r="AH220" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="53"/>
         <v>4</v>
       </c>
     </row>
@@ -17722,119 +18026,119 @@
         <v>49</v>
       </c>
       <c r="F225" s="1">
-        <f t="shared" ref="F225:AH225" si="41">F229+F228+F227+F226</f>
+        <f t="shared" ref="F225:AH225" si="54">F229+F228+F227+F226</f>
         <v>0</v>
       </c>
       <c r="G225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="H225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="I225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="J225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="K225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="L225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="M225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="N225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="O225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="P225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="R225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="S225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="T225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>2</v>
       </c>
       <c r="U225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>6</v>
       </c>
       <c r="V225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>4</v>
       </c>
       <c r="W225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>4</v>
       </c>
       <c r="X225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>4</v>
       </c>
       <c r="Y225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="Z225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="AA225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>2</v>
       </c>
       <c r="AB225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>6</v>
       </c>
       <c r="AC225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>11</v>
       </c>
       <c r="AD225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="AE225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="AF225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="AG225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="AH225" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="54"/>
         <v>2</v>
       </c>
     </row>
@@ -18244,119 +18548,119 @@
         <v>59604</v>
       </c>
       <c r="F230" s="3">
-        <f t="shared" ref="F230:AH230" si="42">F234+F233+F232+F231</f>
+        <f t="shared" ref="F230:AH230" si="55">F234+F233+F232+F231</f>
         <v>991</v>
       </c>
       <c r="G230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2990</v>
       </c>
       <c r="H230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>3203</v>
       </c>
       <c r="I230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>3067</v>
       </c>
       <c r="J230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2406</v>
       </c>
       <c r="K230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2572</v>
       </c>
       <c r="L230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2789</v>
       </c>
       <c r="M230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>3047</v>
       </c>
       <c r="N230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>3095</v>
       </c>
       <c r="O230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2970</v>
       </c>
       <c r="P230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2893</v>
       </c>
       <c r="Q230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2979</v>
       </c>
       <c r="R230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>3009</v>
       </c>
       <c r="S230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2812</v>
       </c>
       <c r="T230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2783</v>
       </c>
       <c r="U230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2639</v>
       </c>
       <c r="V230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2405</v>
       </c>
       <c r="W230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>2206</v>
       </c>
       <c r="X230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>1910</v>
       </c>
       <c r="Y230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>1722</v>
       </c>
       <c r="Z230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>1251</v>
       </c>
       <c r="AA230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>1039</v>
       </c>
       <c r="AB230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>912</v>
       </c>
       <c r="AC230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>813</v>
       </c>
       <c r="AD230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>876</v>
       </c>
       <c r="AE230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>675</v>
       </c>
       <c r="AF230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>565</v>
       </c>
       <c r="AG230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>550</v>
       </c>
       <c r="AH230" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" si="55"/>
         <v>489</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiunto check probabilità di morte ai dati OPTN
</commit_message>
<xml_diff>
--- a/data/Data_Tansplants_US.xlsx
+++ b/data/Data_Tansplants_US.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE0926EB-6D89-467C-841C-300FA50C6DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE039D8-2120-46F7-BDF9-5396C8675076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -799,8 +799,8 @@
   </sheetPr>
   <dimension ref="A1:AO237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="M116" sqref="M116"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="P118" activeCellId="1" sqref="K114 P118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8663,6 +8663,14 @@
       <c r="J114" t="s">
         <v>9</v>
       </c>
+      <c r="K114">
+        <f>K118+K122+K126+K130</f>
+        <v>1</v>
+      </c>
+      <c r="L114">
+        <f>L118+L122+L126+L130</f>
+        <v>1.0000000000000002</v>
+      </c>
     </row>
     <row r="115" spans="1:13">
       <c r="B115" t="s">
@@ -8688,6 +8696,14 @@
       <c r="J115" t="s">
         <v>16</v>
       </c>
+      <c r="K115">
+        <f>K119+K123+K127+K131</f>
+        <v>1</v>
+      </c>
+      <c r="L115">
+        <f>L119+L123+L127+L131</f>
+        <v>0.99999999999999989</v>
+      </c>
     </row>
     <row r="116" spans="1:13">
       <c r="B116" t="s">
@@ -8713,6 +8729,14 @@
       <c r="J116" t="s">
         <v>17</v>
       </c>
+      <c r="K116">
+        <f>K120+K124+K128+K132</f>
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <f>L120+L124+L128+L132</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:13">
       <c r="B117" t="s">
@@ -8737,6 +8761,14 @@
       <c r="G117" s="34"/>
       <c r="J117" t="s">
         <v>18</v>
+      </c>
+      <c r="K117">
+        <f>K121+K125+K129+K133</f>
+        <v>1</v>
+      </c>
+      <c r="L117">
+        <f>L121+L125+L129+L133</f>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="118" spans="1:13">

</xml_diff>

<commit_message>
Aggiunti tassi e probabilità di ripetere il trapianto (p_success, p_repeat) ai dati di OPTN.
</commit_message>
<xml_diff>
--- a/data/Data_Tansplants_US.xlsx
+++ b/data/Data_Tansplants_US.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE039D8-2120-46F7-BDF9-5396C8675076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{628F8164-228D-435C-82AC-A7409DBC0CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="74">
   <si>
     <t>ORGANI</t>
   </si>
@@ -230,6 +230,27 @@
   <si>
     <t>Died</t>
   </si>
+  <si>
+    <t>RIPETIZ TRAP.</t>
+  </si>
+  <si>
+    <t>All Transplant</t>
+  </si>
+  <si>
+    <t>Primary Transplant</t>
+  </si>
+  <si>
+    <t>Repeat Transplant</t>
+  </si>
+  <si>
+    <t>RIPETIZ. TRAP - TASSI</t>
+  </si>
+  <si>
+    <t>PROBABILITÀ - RIPETIZ.</t>
+  </si>
+  <si>
+    <t>VALORE</t>
+  </si>
 </sst>
 </file>
 
@@ -318,7 +339,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -364,21 +385,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -398,6 +404,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -410,23 +440,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,22 +474,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -480,6 +489,27 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -797,10 +827,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AO237"/>
+  <dimension ref="A1:AO260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="P118" activeCellId="1" sqref="K114 P118"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="J261" sqref="J261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -812,10 +842,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1571,7 +1601,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="8"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1651,10 +1681,10 @@
       <c r="AO8" s="1"/>
     </row>
     <row r="9" spans="1:41">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>1</v>
@@ -4973,10 +5003,10 @@
       </c>
     </row>
     <row r="42" spans="1:40">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="18"/>
       <c r="D42" s="1" t="s">
         <v>1</v>
       </c>
@@ -7587,20 +7617,20 @@
       <c r="AG63" s="5"/>
     </row>
     <row r="65" spans="1:19">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B65" s="22"/>
+      <c r="B65" s="18"/>
       <c r="D65" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I65" s="16" t="s">
+      <c r="I65" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J65" s="17"/>
+      <c r="J65" s="13"/>
       <c r="L65" s="2" t="s">
         <v>20</v>
       </c>
@@ -7941,17 +7971,19 @@
       </c>
     </row>
     <row r="87" spans="1:22">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B87" s="30"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="13"/>
       <c r="I87" t="s">
         <v>23</v>
       </c>
-      <c r="K87" s="28" t="s">
+      <c r="K87" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L87" s="28"/>
+      <c r="L87" s="23"/>
       <c r="N87" t="s">
         <v>25</v>
       </c>
@@ -7966,14 +7998,14 @@
       </c>
     </row>
     <row r="88" spans="1:22">
-      <c r="A88" s="21" t="s">
+      <c r="A88" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B88" s="25"/>
-      <c r="C88" s="21" t="s">
+      <c r="B88" s="33"/>
+      <c r="C88" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D88" s="22"/>
+      <c r="D88" s="34"/>
       <c r="I88" s="4">
         <f>D72</f>
         <v>12375</v>
@@ -8003,11 +8035,11 @@
       <c r="A89" t="s">
         <v>30</v>
       </c>
-      <c r="B89" s="8">
+      <c r="B89" s="7">
         <f>D74/D66</f>
         <v>0.32804111562131721</v>
       </c>
-      <c r="D89" s="8">
+      <c r="D89" s="7">
         <f>L68/L66</f>
         <v>0.370336861152608</v>
       </c>
@@ -8016,11 +8048,11 @@
       <c r="A90" t="s">
         <v>31</v>
       </c>
-      <c r="B90" s="8">
+      <c r="B90" s="7">
         <f>D78/D66</f>
         <v>0.14771600665930898</v>
       </c>
-      <c r="D90" s="8">
+      <c r="D90" s="7">
         <f>L69/L66</f>
         <v>0.11885875397142677</v>
       </c>
@@ -8047,11 +8079,11 @@
       <c r="A91" t="s">
         <v>36</v>
       </c>
-      <c r="B91" s="8">
+      <c r="B91" s="7">
         <f>D82/D66</f>
         <v>3.7753231448399704E-2</v>
       </c>
-      <c r="D91" s="8">
+      <c r="D91" s="7">
         <f>L70/L66</f>
         <v>3.3896521976981502E-2</v>
       </c>
@@ -8084,11 +8116,11 @@
       <c r="A92" t="s">
         <v>37</v>
       </c>
-      <c r="B92" s="8">
+      <c r="B92" s="7">
         <f>D70/D66</f>
         <v>0.48651302867618174</v>
       </c>
-      <c r="D92" s="8">
+      <c r="D92" s="7">
         <f>L67/L66</f>
         <v>0.47690786289898368</v>
       </c>
@@ -8140,11 +8172,11 @@
       </c>
     </row>
     <row r="95" spans="1:22">
-      <c r="B95" s="8">
+      <c r="B95" s="7">
         <f>SUM(B89:B92)</f>
         <v>1.0000233824052076</v>
       </c>
-      <c r="D95" s="8">
+      <c r="D95" s="7">
         <f>SUM(D89:D92)</f>
         <v>0.99999999999999989</v>
       </c>
@@ -8173,7 +8205,7 @@
       <c r="A97" t="s">
         <v>46</v>
       </c>
-      <c r="B97" s="11">
+      <c r="B97" s="9">
         <f>D69/D66</f>
         <v>0.28825361491984508</v>
       </c>
@@ -8206,7 +8238,7 @@
       <c r="A98" t="s">
         <v>47</v>
       </c>
-      <c r="B98" s="11">
+      <c r="B98" s="9">
         <f>D67/D66</f>
         <v>9.9609046184926764E-4</v>
       </c>
@@ -8215,7 +8247,7 @@
       <c r="A99" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B99" s="12">
+      <c r="B99" s="10">
         <f>D68/D66</f>
         <v>0.71075029461830563</v>
       </c>
@@ -8359,7 +8391,7 @@
     </row>
     <row r="102" spans="1:40">
       <c r="A102" s="1"/>
-      <c r="B102" s="12">
+      <c r="B102" s="10">
         <f>SUM(B97:B99)</f>
         <v>1</v>
       </c>
@@ -8599,37 +8631,47 @@
       <c r="AK110" s="5"/>
     </row>
     <row r="112" spans="1:40">
-      <c r="A112" s="16" t="s">
+      <c r="A112" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B112" s="17"/>
+      <c r="B112" s="16"/>
+      <c r="C112" s="16"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+      <c r="J112" s="16"/>
+      <c r="K112" s="16"/>
+      <c r="L112" s="13"/>
     </row>
     <row r="113" spans="1:13">
-      <c r="A113" s="26" t="s">
+      <c r="A113" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B113" s="27"/>
-      <c r="C113" s="14" t="s">
+      <c r="B113" s="22"/>
+      <c r="C113" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D113" s="15" t="s">
+      <c r="D113" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E113" s="7" t="s">
+      <c r="E113" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="F113" s="13" t="s">
+      <c r="F113" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G113" s="31"/>
-      <c r="I113" s="16" t="s">
+      <c r="G113" s="24"/>
+      <c r="I113" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="J113" s="20"/>
-      <c r="K113" s="9" t="s">
+      <c r="J113" s="22"/>
+      <c r="K113" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L113" s="14" t="s">
+      <c r="L113" s="28" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8644,7 +8686,7 @@
         <f>AVERAGE(L138:Q138)</f>
         <v>32282.833333333332</v>
       </c>
-      <c r="D114" s="32">
+      <c r="D114" s="25">
         <f>AVERAGE(M206:R206)</f>
         <v>4787</v>
       </c>
@@ -8656,7 +8698,7 @@
         <f>AVERAGE(M172:R172)</f>
         <v>11707.166666666666</v>
       </c>
-      <c r="G114" s="33"/>
+      <c r="G114" s="26"/>
       <c r="I114" t="s">
         <v>3</v>
       </c>
@@ -8692,7 +8734,7 @@
         <f>SUM(AVERAGE(M186:R186),AVERAGE(M191:R191))</f>
         <v>20.833333333333332</v>
       </c>
-      <c r="G115" s="34"/>
+      <c r="G115" s="27"/>
       <c r="J115" t="s">
         <v>16</v>
       </c>
@@ -8725,7 +8767,7 @@
         <f>SUM(AVERAGE(M177:R177),AVERAGE(M181:R181))</f>
         <v>11679.666666666666</v>
       </c>
-      <c r="G116" s="34"/>
+      <c r="G116" s="27"/>
       <c r="J116" t="s">
         <v>17</v>
       </c>
@@ -8758,7 +8800,7 @@
         <f>AVERAGE(M196:R196)</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="G117" s="34"/>
+      <c r="G117" s="27"/>
       <c r="J117" t="s">
         <v>18</v>
       </c>
@@ -9336,10 +9378,10 @@
       <c r="Y135" s="4"/>
     </row>
     <row r="137" spans="1:35">
-      <c r="A137" s="16" t="s">
+      <c r="A137" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B137" s="17"/>
+      <c r="B137" s="13"/>
       <c r="D137" s="1" t="s">
         <v>1</v>
       </c>
@@ -12747,10 +12789,10 @@
       <c r="AI168" s="1"/>
     </row>
     <row r="171" spans="1:35">
-      <c r="A171" s="16" t="s">
+      <c r="A171" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B171" s="17"/>
+      <c r="B171" s="13"/>
       <c r="E171" s="1" t="s">
         <v>1</v>
       </c>
@@ -15835,10 +15877,10 @@
       <c r="P203" s="6"/>
     </row>
     <row r="205" spans="1:34">
-      <c r="A205" s="18" t="s">
+      <c r="A205" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B205" s="19"/>
+      <c r="B205" s="15"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
       <c r="E205" s="1" t="s">
@@ -18044,7 +18086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:34">
+    <row r="225" spans="1:40">
       <c r="A225" s="1"/>
       <c r="B225" s="1" t="s">
         <v>13</v>
@@ -18174,7 +18216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:34">
+    <row r="226" spans="1:40">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1" t="s">
@@ -18272,7 +18314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:34">
+    <row r="227" spans="1:40">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1" t="s">
@@ -18370,7 +18412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:34">
+    <row r="228" spans="1:40">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1" t="s">
@@ -18468,7 +18510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:34">
+    <row r="229" spans="1:40">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1" t="s">
@@ -18566,7 +18608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:34">
+    <row r="230" spans="1:40">
       <c r="A230" s="1"/>
       <c r="B230" s="1" t="s">
         <v>14</v>
@@ -18696,7 +18738,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="231" spans="1:34">
+    <row r="231" spans="1:40">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1" t="s">
@@ -18794,7 +18836,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="232" spans="1:34">
+    <row r="232" spans="1:40">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1" t="s">
@@ -18892,7 +18934,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="233" spans="1:34">
+    <row r="233" spans="1:40">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1" t="s">
@@ -18990,7 +19032,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="234" spans="1:34">
+    <row r="234" spans="1:40">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1" t="s">
@@ -19088,23 +19130,2272 @@
         <v>18</v>
       </c>
     </row>
-    <row r="237" spans="1:34">
-      <c r="K237" s="4"/>
-      <c r="L237" s="4"/>
-      <c r="M237" s="4"/>
-      <c r="N237" s="4"/>
-      <c r="O237" s="4"/>
-      <c r="P237" s="4"/>
-      <c r="Q237" s="4"/>
-      <c r="R237" s="4"/>
+    <row r="237" spans="1:40">
+      <c r="A237" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B237" s="15"/>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E237" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F237" s="1">
+        <v>2022</v>
+      </c>
+      <c r="G237" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H237" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I237" s="1">
+        <v>2019</v>
+      </c>
+      <c r="J237" s="1">
+        <v>2018</v>
+      </c>
+      <c r="K237" s="1">
+        <v>2017</v>
+      </c>
+      <c r="L237" s="1">
+        <v>2016</v>
+      </c>
+      <c r="M237" s="1">
+        <v>2015</v>
+      </c>
+      <c r="N237" s="1">
+        <v>2014</v>
+      </c>
+      <c r="O237" s="1">
+        <v>2013</v>
+      </c>
+      <c r="P237" s="1">
+        <v>2012</v>
+      </c>
+      <c r="Q237" s="1">
+        <v>2011</v>
+      </c>
+      <c r="R237" s="1">
+        <v>2010</v>
+      </c>
+      <c r="S237" s="1">
+        <v>2009</v>
+      </c>
+      <c r="T237" s="1">
+        <v>2008</v>
+      </c>
+      <c r="U237" s="1">
+        <v>2007</v>
+      </c>
+      <c r="V237" s="1">
+        <v>2006</v>
+      </c>
+      <c r="W237" s="1">
+        <v>2005</v>
+      </c>
+      <c r="X237" s="1">
+        <v>2004</v>
+      </c>
+      <c r="Y237" s="1">
+        <v>2003</v>
+      </c>
+      <c r="Z237" s="1">
+        <v>2002</v>
+      </c>
+      <c r="AA237" s="1">
+        <v>2001</v>
+      </c>
+      <c r="AB237" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AC237" s="1">
+        <v>1999</v>
+      </c>
+      <c r="AD237" s="1">
+        <v>1998</v>
+      </c>
+      <c r="AE237" s="1">
+        <v>1997</v>
+      </c>
+      <c r="AF237" s="1">
+        <v>1996</v>
+      </c>
+      <c r="AG237" s="1">
+        <v>1995</v>
+      </c>
+      <c r="AH237" s="1">
+        <v>1994</v>
+      </c>
+      <c r="AI237" s="1">
+        <v>1993</v>
+      </c>
+      <c r="AJ237" s="1">
+        <v>1992</v>
+      </c>
+      <c r="AK237" s="1">
+        <v>1991</v>
+      </c>
+      <c r="AL237" s="1">
+        <v>1990</v>
+      </c>
+      <c r="AM237" s="1">
+        <v>1989</v>
+      </c>
+      <c r="AN237" s="1">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="238" spans="1:40">
+      <c r="A238" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C238" s="1"/>
+      <c r="D238" s="3">
+        <f>SUM(D240,D239)</f>
+        <v>553885</v>
+      </c>
+      <c r="E238" s="3">
+        <f t="shared" ref="E238:AN238" si="56">SUM(E240,E239)</f>
+        <v>11157</v>
+      </c>
+      <c r="F238" s="3">
+        <f t="shared" si="56"/>
+        <v>25500</v>
+      </c>
+      <c r="G238" s="3">
+        <f t="shared" si="56"/>
+        <v>24670</v>
+      </c>
+      <c r="H238" s="3">
+        <f t="shared" si="56"/>
+        <v>22817</v>
+      </c>
+      <c r="I238" s="3">
+        <f t="shared" si="56"/>
+        <v>23401</v>
+      </c>
+      <c r="J238" s="3">
+        <f t="shared" si="56"/>
+        <v>21167</v>
+      </c>
+      <c r="K238" s="3">
+        <f t="shared" si="56"/>
+        <v>19849</v>
+      </c>
+      <c r="L238" s="3">
+        <f t="shared" si="56"/>
+        <v>19060</v>
+      </c>
+      <c r="M238" s="3">
+        <f t="shared" si="56"/>
+        <v>17878</v>
+      </c>
+      <c r="N238" s="3">
+        <f t="shared" si="56"/>
+        <v>17108</v>
+      </c>
+      <c r="O238" s="3">
+        <f t="shared" si="56"/>
+        <v>16896</v>
+      </c>
+      <c r="P238" s="3">
+        <f t="shared" si="56"/>
+        <v>16487</v>
+      </c>
+      <c r="Q238" s="3">
+        <f t="shared" si="56"/>
+        <v>16816</v>
+      </c>
+      <c r="R238" s="3">
+        <f t="shared" si="56"/>
+        <v>16900</v>
+      </c>
+      <c r="S238" s="3">
+        <f t="shared" si="56"/>
+        <v>16829</v>
+      </c>
+      <c r="T238" s="3">
+        <f t="shared" si="56"/>
+        <v>16521</v>
+      </c>
+      <c r="U238" s="3">
+        <f t="shared" si="56"/>
+        <v>16634</v>
+      </c>
+      <c r="V238" s="3">
+        <f t="shared" si="56"/>
+        <v>17095</v>
+      </c>
+      <c r="W238" s="3">
+        <f t="shared" si="56"/>
+        <v>16485</v>
+      </c>
+      <c r="X238" s="3">
+        <f t="shared" si="56"/>
+        <v>16007</v>
+      </c>
+      <c r="Y238" s="3">
+        <f t="shared" si="56"/>
+        <v>15138</v>
+      </c>
+      <c r="Z238" s="3">
+        <f t="shared" si="56"/>
+        <v>14781</v>
+      </c>
+      <c r="AA238" s="3">
+        <f t="shared" si="56"/>
+        <v>14279</v>
+      </c>
+      <c r="AB238" s="3">
+        <f t="shared" si="56"/>
+        <v>13631</v>
+      </c>
+      <c r="AC238" s="3">
+        <f t="shared" si="56"/>
+        <v>12765</v>
+      </c>
+      <c r="AD238" s="3">
+        <f t="shared" si="56"/>
+        <v>12451</v>
+      </c>
+      <c r="AE238" s="3">
+        <f t="shared" si="56"/>
+        <v>11710</v>
+      </c>
+      <c r="AF238" s="3">
+        <f t="shared" si="56"/>
+        <v>11411</v>
+      </c>
+      <c r="AG238" s="3">
+        <f t="shared" si="56"/>
+        <v>11084</v>
+      </c>
+      <c r="AH238" s="3">
+        <f t="shared" si="56"/>
+        <v>10646</v>
+      </c>
+      <c r="AI238" s="3">
+        <f t="shared" si="56"/>
+        <v>10360</v>
+      </c>
+      <c r="AJ238" s="3">
+        <f t="shared" si="56"/>
+        <v>9738</v>
+      </c>
+      <c r="AK238" s="3">
+        <f t="shared" si="56"/>
+        <v>9677</v>
+      </c>
+      <c r="AL238" s="3">
+        <f t="shared" si="56"/>
+        <v>9405</v>
+      </c>
+      <c r="AM238" s="3">
+        <f t="shared" si="56"/>
+        <v>8655</v>
+      </c>
+      <c r="AN238" s="3">
+        <f t="shared" si="56"/>
+        <v>8877</v>
+      </c>
+    </row>
+    <row r="239" spans="1:40">
+      <c r="A239" s="1"/>
+      <c r="B239" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C239" s="1"/>
+      <c r="D239" s="3">
+        <f>SUM(D242,D245,D248,D251)</f>
+        <v>488019</v>
+      </c>
+      <c r="E239" s="3">
+        <f t="shared" ref="E239:AN239" si="57">SUM(E242,E245,E248,E251)</f>
+        <v>10003</v>
+      </c>
+      <c r="F239" s="3">
+        <f t="shared" si="57"/>
+        <v>23175</v>
+      </c>
+      <c r="G239" s="3">
+        <f t="shared" si="57"/>
+        <v>22196</v>
+      </c>
+      <c r="H239" s="3">
+        <f t="shared" si="57"/>
+        <v>20642</v>
+      </c>
+      <c r="I239" s="3">
+        <f t="shared" si="57"/>
+        <v>20993</v>
+      </c>
+      <c r="J239" s="3">
+        <f t="shared" si="57"/>
+        <v>18973</v>
+      </c>
+      <c r="K239" s="3">
+        <f t="shared" si="57"/>
+        <v>17583</v>
+      </c>
+      <c r="L239" s="3">
+        <f t="shared" si="57"/>
+        <v>16705</v>
+      </c>
+      <c r="M239" s="3">
+        <f t="shared" si="57"/>
+        <v>15554</v>
+      </c>
+      <c r="N239" s="3">
+        <f t="shared" si="57"/>
+        <v>15098</v>
+      </c>
+      <c r="O239" s="3">
+        <f t="shared" si="57"/>
+        <v>14965</v>
+      </c>
+      <c r="P239" s="3">
+        <f t="shared" si="57"/>
+        <v>14498</v>
+      </c>
+      <c r="Q239" s="3">
+        <f t="shared" si="57"/>
+        <v>14909</v>
+      </c>
+      <c r="R239" s="3">
+        <f t="shared" si="57"/>
+        <v>14954</v>
+      </c>
+      <c r="S239" s="3">
+        <f t="shared" si="57"/>
+        <v>14868</v>
+      </c>
+      <c r="T239" s="3">
+        <f t="shared" si="57"/>
+        <v>14751</v>
+      </c>
+      <c r="U239" s="3">
+        <f t="shared" si="57"/>
+        <v>14814</v>
+      </c>
+      <c r="V239" s="3">
+        <f t="shared" si="57"/>
+        <v>15112</v>
+      </c>
+      <c r="W239" s="3">
+        <f t="shared" si="57"/>
+        <v>14568</v>
+      </c>
+      <c r="X239" s="3">
+        <f t="shared" si="57"/>
+        <v>14099</v>
+      </c>
+      <c r="Y239" s="3">
+        <f t="shared" si="57"/>
+        <v>13343</v>
+      </c>
+      <c r="Z239" s="3">
+        <f t="shared" si="57"/>
+        <v>13015</v>
+      </c>
+      <c r="AA239" s="3">
+        <f t="shared" si="57"/>
+        <v>12549</v>
+      </c>
+      <c r="AB239" s="3">
+        <f t="shared" si="57"/>
+        <v>11959</v>
+      </c>
+      <c r="AC239" s="3">
+        <f t="shared" si="57"/>
+        <v>11300</v>
+      </c>
+      <c r="AD239" s="3">
+        <f t="shared" si="57"/>
+        <v>10971</v>
+      </c>
+      <c r="AE239" s="3">
+        <f t="shared" si="57"/>
+        <v>10324</v>
+      </c>
+      <c r="AF239" s="3">
+        <f t="shared" si="57"/>
+        <v>10046</v>
+      </c>
+      <c r="AG239" s="3">
+        <f t="shared" si="57"/>
+        <v>9734</v>
+      </c>
+      <c r="AH239" s="3">
+        <f t="shared" si="57"/>
+        <v>9325</v>
+      </c>
+      <c r="AI239" s="3">
+        <f t="shared" si="57"/>
+        <v>9025</v>
+      </c>
+      <c r="AJ239" s="3">
+        <f t="shared" si="57"/>
+        <v>8181</v>
+      </c>
+      <c r="AK239" s="3">
+        <f t="shared" si="57"/>
+        <v>7976</v>
+      </c>
+      <c r="AL239" s="3">
+        <f t="shared" si="57"/>
+        <v>7775</v>
+      </c>
+      <c r="AM239" s="3">
+        <f t="shared" si="57"/>
+        <v>7070</v>
+      </c>
+      <c r="AN239" s="3">
+        <f t="shared" si="57"/>
+        <v>6966</v>
+      </c>
+    </row>
+    <row r="240" spans="1:40">
+      <c r="A240" s="1"/>
+      <c r="B240" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C240" s="1"/>
+      <c r="D240" s="3">
+        <f>SUM(D243,D246,D249,D252)</f>
+        <v>65866</v>
+      </c>
+      <c r="E240" s="3">
+        <f t="shared" ref="E240:AN240" si="58">SUM(E243,E246,E249,E252)</f>
+        <v>1154</v>
+      </c>
+      <c r="F240" s="3">
+        <f t="shared" si="58"/>
+        <v>2325</v>
+      </c>
+      <c r="G240" s="3">
+        <f t="shared" si="58"/>
+        <v>2474</v>
+      </c>
+      <c r="H240" s="3">
+        <f t="shared" si="58"/>
+        <v>2175</v>
+      </c>
+      <c r="I240" s="3">
+        <f t="shared" si="58"/>
+        <v>2408</v>
+      </c>
+      <c r="J240" s="3">
+        <f t="shared" si="58"/>
+        <v>2194</v>
+      </c>
+      <c r="K240" s="3">
+        <f t="shared" si="58"/>
+        <v>2266</v>
+      </c>
+      <c r="L240" s="3">
+        <f t="shared" si="58"/>
+        <v>2355</v>
+      </c>
+      <c r="M240" s="3">
+        <f t="shared" si="58"/>
+        <v>2324</v>
+      </c>
+      <c r="N240" s="3">
+        <f t="shared" si="58"/>
+        <v>2010</v>
+      </c>
+      <c r="O240" s="3">
+        <f t="shared" si="58"/>
+        <v>1931</v>
+      </c>
+      <c r="P240" s="3">
+        <f t="shared" si="58"/>
+        <v>1989</v>
+      </c>
+      <c r="Q240" s="3">
+        <f t="shared" si="58"/>
+        <v>1907</v>
+      </c>
+      <c r="R240" s="3">
+        <f t="shared" si="58"/>
+        <v>1946</v>
+      </c>
+      <c r="S240" s="3">
+        <f t="shared" si="58"/>
+        <v>1961</v>
+      </c>
+      <c r="T240" s="3">
+        <f t="shared" si="58"/>
+        <v>1770</v>
+      </c>
+      <c r="U240" s="3">
+        <f t="shared" si="58"/>
+        <v>1820</v>
+      </c>
+      <c r="V240" s="3">
+        <f t="shared" si="58"/>
+        <v>1983</v>
+      </c>
+      <c r="W240" s="3">
+        <f t="shared" si="58"/>
+        <v>1917</v>
+      </c>
+      <c r="X240" s="3">
+        <f t="shared" si="58"/>
+        <v>1908</v>
+      </c>
+      <c r="Y240" s="3">
+        <f t="shared" si="58"/>
+        <v>1795</v>
+      </c>
+      <c r="Z240" s="3">
+        <f t="shared" si="58"/>
+        <v>1766</v>
+      </c>
+      <c r="AA240" s="3">
+        <f t="shared" si="58"/>
+        <v>1730</v>
+      </c>
+      <c r="AB240" s="3">
+        <f t="shared" si="58"/>
+        <v>1672</v>
+      </c>
+      <c r="AC240" s="3">
+        <f t="shared" si="58"/>
+        <v>1465</v>
+      </c>
+      <c r="AD240" s="3">
+        <f t="shared" si="58"/>
+        <v>1480</v>
+      </c>
+      <c r="AE240" s="3">
+        <f t="shared" si="58"/>
+        <v>1386</v>
+      </c>
+      <c r="AF240" s="3">
+        <f t="shared" si="58"/>
+        <v>1365</v>
+      </c>
+      <c r="AG240" s="3">
+        <f t="shared" si="58"/>
+        <v>1350</v>
+      </c>
+      <c r="AH240" s="3">
+        <f t="shared" si="58"/>
+        <v>1321</v>
+      </c>
+      <c r="AI240" s="3">
+        <f t="shared" si="58"/>
+        <v>1335</v>
+      </c>
+      <c r="AJ240" s="3">
+        <f t="shared" si="58"/>
+        <v>1557</v>
+      </c>
+      <c r="AK240" s="3">
+        <f t="shared" si="58"/>
+        <v>1701</v>
+      </c>
+      <c r="AL240" s="3">
+        <f t="shared" si="58"/>
+        <v>1630</v>
+      </c>
+      <c r="AM240" s="3">
+        <f t="shared" si="58"/>
+        <v>1585</v>
+      </c>
+      <c r="AN240" s="3">
+        <f t="shared" si="58"/>
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="241" spans="1:40">
+      <c r="A241" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C241" s="1"/>
+      <c r="D241" s="3">
+        <f>SUM(D243,D242)</f>
+        <v>250146</v>
+      </c>
+      <c r="E241" s="3">
+        <f t="shared" ref="E241:AN241" si="59">SUM(E243,E242)</f>
+        <v>5137</v>
+      </c>
+      <c r="F241" s="3">
+        <f t="shared" si="59"/>
+        <v>11725</v>
+      </c>
+      <c r="G241" s="3">
+        <f t="shared" si="59"/>
+        <v>11359</v>
+      </c>
+      <c r="H241" s="3">
+        <f t="shared" si="59"/>
+        <v>10393</v>
+      </c>
+      <c r="I241" s="3">
+        <f t="shared" si="59"/>
+        <v>10616</v>
+      </c>
+      <c r="J241" s="3">
+        <f t="shared" si="59"/>
+        <v>9523</v>
+      </c>
+      <c r="K241" s="3">
+        <f t="shared" si="59"/>
+        <v>8995</v>
+      </c>
+      <c r="L241" s="3">
+        <f t="shared" si="59"/>
+        <v>8612</v>
+      </c>
+      <c r="M241" s="3">
+        <f t="shared" si="59"/>
+        <v>8088</v>
+      </c>
+      <c r="N241" s="3">
+        <f t="shared" si="59"/>
+        <v>7659</v>
+      </c>
+      <c r="O241" s="3">
+        <f t="shared" si="59"/>
+        <v>7631</v>
+      </c>
+      <c r="P241" s="3">
+        <f t="shared" si="59"/>
+        <v>7314</v>
+      </c>
+      <c r="Q241" s="3">
+        <f t="shared" si="59"/>
+        <v>7606</v>
+      </c>
+      <c r="R241" s="3">
+        <f t="shared" si="59"/>
+        <v>7637</v>
+      </c>
+      <c r="S241" s="3">
+        <f t="shared" si="59"/>
+        <v>7604</v>
+      </c>
+      <c r="T241" s="3">
+        <f t="shared" si="59"/>
+        <v>7336</v>
+      </c>
+      <c r="U241" s="3">
+        <f t="shared" si="59"/>
+        <v>7606</v>
+      </c>
+      <c r="V241" s="3">
+        <f t="shared" si="59"/>
+        <v>7665</v>
+      </c>
+      <c r="W241" s="3">
+        <f t="shared" si="59"/>
+        <v>7407</v>
+      </c>
+      <c r="X241" s="3">
+        <f t="shared" si="59"/>
+        <v>7312</v>
+      </c>
+      <c r="Y241" s="3">
+        <f t="shared" si="59"/>
+        <v>6948</v>
+      </c>
+      <c r="Z241" s="3">
+        <f t="shared" si="59"/>
+        <v>6631</v>
+      </c>
+      <c r="AA241" s="3">
+        <f t="shared" si="59"/>
+        <v>6401</v>
+      </c>
+      <c r="AB241" s="3">
+        <f t="shared" si="59"/>
+        <v>6129</v>
+      </c>
+      <c r="AC241" s="3">
+        <f t="shared" si="59"/>
+        <v>5543</v>
+      </c>
+      <c r="AD241" s="3">
+        <f t="shared" si="59"/>
+        <v>5546</v>
+      </c>
+      <c r="AE241" s="3">
+        <f t="shared" si="59"/>
+        <v>5139</v>
+      </c>
+      <c r="AF241" s="3">
+        <f t="shared" si="59"/>
+        <v>5077</v>
+      </c>
+      <c r="AG241" s="3">
+        <f t="shared" si="59"/>
+        <v>4936</v>
+      </c>
+      <c r="AH241" s="3">
+        <f t="shared" si="59"/>
+        <v>4860</v>
+      </c>
+      <c r="AI241" s="3">
+        <f t="shared" si="59"/>
+        <v>4660</v>
+      </c>
+      <c r="AJ241" s="3">
+        <f t="shared" si="59"/>
+        <v>4505</v>
+      </c>
+      <c r="AK241" s="3">
+        <f t="shared" si="59"/>
+        <v>4366</v>
+      </c>
+      <c r="AL241" s="3">
+        <f t="shared" si="59"/>
+        <v>4172</v>
+      </c>
+      <c r="AM241" s="3">
+        <f t="shared" si="59"/>
+        <v>3968</v>
+      </c>
+      <c r="AN241" s="3">
+        <f t="shared" si="59"/>
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="242" spans="1:40">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C242" s="1"/>
+      <c r="D242" s="3">
+        <v>220798</v>
+      </c>
+      <c r="E242" s="3">
+        <v>4623</v>
+      </c>
+      <c r="F242" s="3">
+        <v>10630</v>
+      </c>
+      <c r="G242" s="3">
+        <v>10238</v>
+      </c>
+      <c r="H242" s="3">
+        <v>9386</v>
+      </c>
+      <c r="I242" s="3">
+        <v>9509</v>
+      </c>
+      <c r="J242" s="3">
+        <v>8558</v>
+      </c>
+      <c r="K242" s="3">
+        <v>7941</v>
+      </c>
+      <c r="L242" s="3">
+        <v>7510</v>
+      </c>
+      <c r="M242" s="3">
+        <v>6968</v>
+      </c>
+      <c r="N242" s="3">
+        <v>6754</v>
+      </c>
+      <c r="O242" s="3">
+        <v>6741</v>
+      </c>
+      <c r="P242" s="3">
+        <v>6443</v>
+      </c>
+      <c r="Q242" s="3">
+        <v>6760</v>
+      </c>
+      <c r="R242" s="3">
+        <v>6741</v>
+      </c>
+      <c r="S242" s="3">
+        <v>6750</v>
+      </c>
+      <c r="T242" s="3">
+        <v>6565</v>
+      </c>
+      <c r="U242" s="3">
+        <v>6834</v>
+      </c>
+      <c r="V242" s="3">
+        <v>6802</v>
+      </c>
+      <c r="W242" s="3">
+        <v>6553</v>
+      </c>
+      <c r="X242" s="3">
+        <v>6406</v>
+      </c>
+      <c r="Y242" s="3">
+        <v>6123</v>
+      </c>
+      <c r="Z242" s="3">
+        <v>5882</v>
+      </c>
+      <c r="AA242" s="3">
+        <v>5616</v>
+      </c>
+      <c r="AB242" s="3">
+        <v>5398</v>
+      </c>
+      <c r="AC242" s="3">
+        <v>4938</v>
+      </c>
+      <c r="AD242" s="3">
+        <v>4917</v>
+      </c>
+      <c r="AE242" s="3">
+        <v>4571</v>
+      </c>
+      <c r="AF242" s="3">
+        <v>4482</v>
+      </c>
+      <c r="AG242" s="3">
+        <v>4377</v>
+      </c>
+      <c r="AH242" s="3">
+        <v>4291</v>
+      </c>
+      <c r="AI242" s="3">
+        <v>4093</v>
+      </c>
+      <c r="AJ242" s="3">
+        <v>3825</v>
+      </c>
+      <c r="AK242" s="3">
+        <v>3614</v>
+      </c>
+      <c r="AL242" s="3">
+        <v>3474</v>
+      </c>
+      <c r="AM242" s="3">
+        <v>3288</v>
+      </c>
+      <c r="AN242" s="3">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="243" spans="1:40">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C243" s="1"/>
+      <c r="D243" s="3">
+        <v>29348</v>
+      </c>
+      <c r="E243" s="1">
+        <v>514</v>
+      </c>
+      <c r="F243" s="3">
+        <v>1095</v>
+      </c>
+      <c r="G243" s="3">
+        <v>1121</v>
+      </c>
+      <c r="H243" s="3">
+        <v>1007</v>
+      </c>
+      <c r="I243" s="3">
+        <v>1107</v>
+      </c>
+      <c r="J243" s="1">
+        <v>965</v>
+      </c>
+      <c r="K243" s="3">
+        <v>1054</v>
+      </c>
+      <c r="L243" s="3">
+        <v>1102</v>
+      </c>
+      <c r="M243" s="3">
+        <v>1120</v>
+      </c>
+      <c r="N243" s="1">
+        <v>905</v>
+      </c>
+      <c r="O243" s="1">
+        <v>890</v>
+      </c>
+      <c r="P243" s="1">
+        <v>871</v>
+      </c>
+      <c r="Q243" s="1">
+        <v>846</v>
+      </c>
+      <c r="R243" s="1">
+        <v>896</v>
+      </c>
+      <c r="S243" s="1">
+        <v>854</v>
+      </c>
+      <c r="T243" s="1">
+        <v>771</v>
+      </c>
+      <c r="U243" s="1">
+        <v>772</v>
+      </c>
+      <c r="V243" s="1">
+        <v>863</v>
+      </c>
+      <c r="W243" s="1">
+        <v>854</v>
+      </c>
+      <c r="X243" s="1">
+        <v>906</v>
+      </c>
+      <c r="Y243" s="1">
+        <v>825</v>
+      </c>
+      <c r="Z243" s="1">
+        <v>749</v>
+      </c>
+      <c r="AA243" s="1">
+        <v>785</v>
+      </c>
+      <c r="AB243" s="1">
+        <v>731</v>
+      </c>
+      <c r="AC243" s="1">
+        <v>605</v>
+      </c>
+      <c r="AD243" s="1">
+        <v>629</v>
+      </c>
+      <c r="AE243" s="1">
+        <v>568</v>
+      </c>
+      <c r="AF243" s="1">
+        <v>595</v>
+      </c>
+      <c r="AG243" s="1">
+        <v>559</v>
+      </c>
+      <c r="AH243" s="1">
+        <v>569</v>
+      </c>
+      <c r="AI243" s="1">
+        <v>567</v>
+      </c>
+      <c r="AJ243" s="1">
+        <v>680</v>
+      </c>
+      <c r="AK243" s="1">
+        <v>752</v>
+      </c>
+      <c r="AL243" s="1">
+        <v>698</v>
+      </c>
+      <c r="AM243" s="1">
+        <v>680</v>
+      </c>
+      <c r="AN243" s="1">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="244" spans="1:40">
+      <c r="A244" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C244" s="1"/>
+      <c r="D244" s="3">
+        <f>SUM(D246,D245)</f>
+        <v>205213</v>
+      </c>
+      <c r="E244" s="3">
+        <f t="shared" ref="E244:AN244" si="60">SUM(E246,E245)</f>
+        <v>3870</v>
+      </c>
+      <c r="F244" s="3">
+        <f t="shared" si="60"/>
+        <v>8864</v>
+      </c>
+      <c r="G244" s="3">
+        <f t="shared" si="60"/>
+        <v>8678</v>
+      </c>
+      <c r="H244" s="3">
+        <f t="shared" si="60"/>
+        <v>8180</v>
+      </c>
+      <c r="I244" s="3">
+        <f t="shared" si="60"/>
+        <v>8372</v>
+      </c>
+      <c r="J244" s="3">
+        <f t="shared" si="60"/>
+        <v>7553</v>
+      </c>
+      <c r="K244" s="3">
+        <f t="shared" si="60"/>
+        <v>7214</v>
+      </c>
+      <c r="L244" s="3">
+        <f t="shared" si="60"/>
+        <v>7001</v>
+      </c>
+      <c r="M244" s="3">
+        <f t="shared" si="60"/>
+        <v>6470</v>
+      </c>
+      <c r="N244" s="3">
+        <f t="shared" si="60"/>
+        <v>6364</v>
+      </c>
+      <c r="O244" s="3">
+        <f t="shared" si="60"/>
+        <v>6254</v>
+      </c>
+      <c r="P244" s="3">
+        <f t="shared" si="60"/>
+        <v>6150</v>
+      </c>
+      <c r="Q244" s="3">
+        <f t="shared" si="60"/>
+        <v>6227</v>
+      </c>
+      <c r="R244" s="3">
+        <f t="shared" si="60"/>
+        <v>6124</v>
+      </c>
+      <c r="S244" s="3">
+        <f t="shared" si="60"/>
+        <v>6236</v>
+      </c>
+      <c r="T244" s="3">
+        <f t="shared" si="60"/>
+        <v>6158</v>
+      </c>
+      <c r="U244" s="3">
+        <f t="shared" si="60"/>
+        <v>6117</v>
+      </c>
+      <c r="V244" s="3">
+        <f t="shared" si="60"/>
+        <v>6354</v>
+      </c>
+      <c r="W244" s="3">
+        <f t="shared" si="60"/>
+        <v>6187</v>
+      </c>
+      <c r="X244" s="3">
+        <f t="shared" si="60"/>
+        <v>5931</v>
+      </c>
+      <c r="Y244" s="3">
+        <f t="shared" si="60"/>
+        <v>5635</v>
+      </c>
+      <c r="Z244" s="3">
+        <f t="shared" si="60"/>
+        <v>5610</v>
+      </c>
+      <c r="AA244" s="3">
+        <f t="shared" si="60"/>
+        <v>5466</v>
+      </c>
+      <c r="AB244" s="3">
+        <f t="shared" si="60"/>
+        <v>5216</v>
+      </c>
+      <c r="AC244" s="3">
+        <f t="shared" si="60"/>
+        <v>4925</v>
+      </c>
+      <c r="AD244" s="3">
+        <f t="shared" si="60"/>
+        <v>4768</v>
+      </c>
+      <c r="AE244" s="3">
+        <f t="shared" si="60"/>
+        <v>4586</v>
+      </c>
+      <c r="AF244" s="3">
+        <f t="shared" si="60"/>
+        <v>4474</v>
+      </c>
+      <c r="AG244" s="3">
+        <f t="shared" si="60"/>
+        <v>4292</v>
+      </c>
+      <c r="AH244" s="3">
+        <f t="shared" si="60"/>
+        <v>4046</v>
+      </c>
+      <c r="AI244" s="3">
+        <f t="shared" si="60"/>
+        <v>4060</v>
+      </c>
+      <c r="AJ244" s="3">
+        <f t="shared" si="60"/>
+        <v>3674</v>
+      </c>
+      <c r="AK244" s="3">
+        <f t="shared" si="60"/>
+        <v>3760</v>
+      </c>
+      <c r="AL244" s="3">
+        <f t="shared" si="60"/>
+        <v>3721</v>
+      </c>
+      <c r="AM244" s="3">
+        <f t="shared" si="60"/>
+        <v>3263</v>
+      </c>
+      <c r="AN244" s="3">
+        <f t="shared" si="60"/>
+        <v>3413</v>
+      </c>
+    </row>
+    <row r="245" spans="1:40">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C245" s="1"/>
+      <c r="D245" s="3">
+        <v>179246</v>
+      </c>
+      <c r="E245" s="3">
+        <v>3431</v>
+      </c>
+      <c r="F245" s="3">
+        <v>8042</v>
+      </c>
+      <c r="G245" s="3">
+        <v>7745</v>
+      </c>
+      <c r="H245" s="3">
+        <v>7380</v>
+      </c>
+      <c r="I245" s="3">
+        <v>7491</v>
+      </c>
+      <c r="J245" s="3">
+        <v>6720</v>
+      </c>
+      <c r="K245" s="3">
+        <v>6370</v>
+      </c>
+      <c r="L245" s="3">
+        <v>6098</v>
+      </c>
+      <c r="M245" s="3">
+        <v>5617</v>
+      </c>
+      <c r="N245" s="3">
+        <v>5571</v>
+      </c>
+      <c r="O245" s="3">
+        <v>5514</v>
+      </c>
+      <c r="P245" s="3">
+        <v>5355</v>
+      </c>
+      <c r="Q245" s="3">
+        <v>5473</v>
+      </c>
+      <c r="R245" s="3">
+        <v>5408</v>
+      </c>
+      <c r="S245" s="3">
+        <v>5444</v>
+      </c>
+      <c r="T245" s="3">
+        <v>5425</v>
+      </c>
+      <c r="U245" s="3">
+        <v>5367</v>
+      </c>
+      <c r="V245" s="3">
+        <v>5563</v>
+      </c>
+      <c r="W245" s="3">
+        <v>5433</v>
+      </c>
+      <c r="X245" s="3">
+        <v>5202</v>
+      </c>
+      <c r="Y245" s="3">
+        <v>4946</v>
+      </c>
+      <c r="Z245" s="3">
+        <v>4892</v>
+      </c>
+      <c r="AA245" s="3">
+        <v>4787</v>
+      </c>
+      <c r="AB245" s="3">
+        <v>4532</v>
+      </c>
+      <c r="AC245" s="3">
+        <v>4331</v>
+      </c>
+      <c r="AD245" s="3">
+        <v>4117</v>
+      </c>
+      <c r="AE245" s="3">
+        <v>3992</v>
+      </c>
+      <c r="AF245" s="3">
+        <v>3902</v>
+      </c>
+      <c r="AG245" s="3">
+        <v>3713</v>
+      </c>
+      <c r="AH245" s="3">
+        <v>3484</v>
+      </c>
+      <c r="AI245" s="3">
+        <v>3515</v>
+      </c>
+      <c r="AJ245" s="3">
+        <v>3028</v>
+      </c>
+      <c r="AK245" s="3">
+        <v>3065</v>
+      </c>
+      <c r="AL245" s="3">
+        <v>3027</v>
+      </c>
+      <c r="AM245" s="3">
+        <v>2624</v>
+      </c>
+      <c r="AN245" s="3">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="246" spans="1:40">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C246" s="1"/>
+      <c r="D246" s="3">
+        <v>25967</v>
+      </c>
+      <c r="E246" s="1">
+        <v>439</v>
+      </c>
+      <c r="F246" s="1">
+        <v>822</v>
+      </c>
+      <c r="G246" s="1">
+        <v>933</v>
+      </c>
+      <c r="H246" s="1">
+        <v>800</v>
+      </c>
+      <c r="I246" s="1">
+        <v>881</v>
+      </c>
+      <c r="J246" s="1">
+        <v>833</v>
+      </c>
+      <c r="K246" s="1">
+        <v>844</v>
+      </c>
+      <c r="L246" s="1">
+        <v>903</v>
+      </c>
+      <c r="M246" s="1">
+        <v>853</v>
+      </c>
+      <c r="N246" s="1">
+        <v>793</v>
+      </c>
+      <c r="O246" s="1">
+        <v>740</v>
+      </c>
+      <c r="P246" s="1">
+        <v>795</v>
+      </c>
+      <c r="Q246" s="1">
+        <v>754</v>
+      </c>
+      <c r="R246" s="1">
+        <v>716</v>
+      </c>
+      <c r="S246" s="1">
+        <v>792</v>
+      </c>
+      <c r="T246" s="1">
+        <v>733</v>
+      </c>
+      <c r="U246" s="1">
+        <v>750</v>
+      </c>
+      <c r="V246" s="1">
+        <v>791</v>
+      </c>
+      <c r="W246" s="1">
+        <v>754</v>
+      </c>
+      <c r="X246" s="1">
+        <v>729</v>
+      </c>
+      <c r="Y246" s="1">
+        <v>689</v>
+      </c>
+      <c r="Z246" s="1">
+        <v>718</v>
+      </c>
+      <c r="AA246" s="1">
+        <v>679</v>
+      </c>
+      <c r="AB246" s="1">
+        <v>684</v>
+      </c>
+      <c r="AC246" s="1">
+        <v>594</v>
+      </c>
+      <c r="AD246" s="1">
+        <v>651</v>
+      </c>
+      <c r="AE246" s="1">
+        <v>594</v>
+      </c>
+      <c r="AF246" s="1">
+        <v>572</v>
+      </c>
+      <c r="AG246" s="1">
+        <v>579</v>
+      </c>
+      <c r="AH246" s="1">
+        <v>562</v>
+      </c>
+      <c r="AI246" s="1">
+        <v>545</v>
+      </c>
+      <c r="AJ246" s="1">
+        <v>646</v>
+      </c>
+      <c r="AK246" s="1">
+        <v>695</v>
+      </c>
+      <c r="AL246" s="1">
+        <v>694</v>
+      </c>
+      <c r="AM246" s="1">
+        <v>639</v>
+      </c>
+      <c r="AN246" s="1">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="247" spans="1:40">
+      <c r="A247" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C247" s="1"/>
+      <c r="D247" s="3">
+        <f>SUM(D249,D248)</f>
+        <v>72371</v>
+      </c>
+      <c r="E247" s="3">
+        <f t="shared" ref="E247:AN247" si="61">SUM(E249,E248)</f>
+        <v>1627</v>
+      </c>
+      <c r="F247" s="3">
+        <f t="shared" si="61"/>
+        <v>3709</v>
+      </c>
+      <c r="G247" s="3">
+        <f t="shared" si="61"/>
+        <v>3531</v>
+      </c>
+      <c r="H247" s="3">
+        <f t="shared" si="61"/>
+        <v>3194</v>
+      </c>
+      <c r="I247" s="3">
+        <f t="shared" si="61"/>
+        <v>3233</v>
+      </c>
+      <c r="J247" s="3">
+        <f t="shared" si="61"/>
+        <v>3061</v>
+      </c>
+      <c r="K247" s="3">
+        <f t="shared" si="61"/>
+        <v>2672</v>
+      </c>
+      <c r="L247" s="3">
+        <f t="shared" si="61"/>
+        <v>2587</v>
+      </c>
+      <c r="M247" s="3">
+        <f t="shared" si="61"/>
+        <v>2366</v>
+      </c>
+      <c r="N247" s="3">
+        <f t="shared" si="61"/>
+        <v>2284</v>
+      </c>
+      <c r="O247" s="3">
+        <f t="shared" si="61"/>
+        <v>2196</v>
+      </c>
+      <c r="P247" s="3">
+        <f t="shared" si="61"/>
+        <v>2164</v>
+      </c>
+      <c r="Q247" s="3">
+        <f t="shared" si="61"/>
+        <v>2164</v>
+      </c>
+      <c r="R247" s="3">
+        <f t="shared" si="61"/>
+        <v>2314</v>
+      </c>
+      <c r="S247" s="3">
+        <f t="shared" si="61"/>
+        <v>2191</v>
+      </c>
+      <c r="T247" s="3">
+        <f t="shared" si="61"/>
+        <v>2259</v>
+      </c>
+      <c r="U247" s="3">
+        <f t="shared" si="61"/>
+        <v>2083</v>
+      </c>
+      <c r="V247" s="3">
+        <f t="shared" si="61"/>
+        <v>2254</v>
+      </c>
+      <c r="W247" s="3">
+        <f t="shared" si="61"/>
+        <v>2121</v>
+      </c>
+      <c r="X247" s="3">
+        <f t="shared" si="61"/>
+        <v>2064</v>
+      </c>
+      <c r="Y247" s="3">
+        <f t="shared" si="61"/>
+        <v>1887</v>
+      </c>
+      <c r="Z247" s="3">
+        <f t="shared" si="61"/>
+        <v>1847</v>
+      </c>
+      <c r="AA247" s="3">
+        <f t="shared" si="61"/>
+        <v>1745</v>
+      </c>
+      <c r="AB247" s="3">
+        <f t="shared" si="61"/>
+        <v>1661</v>
+      </c>
+      <c r="AC247" s="3">
+        <f t="shared" si="61"/>
+        <v>1663</v>
+      </c>
+      <c r="AD247" s="3">
+        <f t="shared" si="61"/>
+        <v>1568</v>
+      </c>
+      <c r="AE247" s="3">
+        <f t="shared" si="61"/>
+        <v>1459</v>
+      </c>
+      <c r="AF247" s="3">
+        <f t="shared" si="61"/>
+        <v>1322</v>
+      </c>
+      <c r="AG247" s="3">
+        <f t="shared" si="61"/>
+        <v>1320</v>
+      </c>
+      <c r="AH247" s="3">
+        <f t="shared" si="61"/>
+        <v>1236</v>
+      </c>
+      <c r="AI247" s="3">
+        <f t="shared" si="61"/>
+        <v>1214</v>
+      </c>
+      <c r="AJ247" s="3">
+        <f t="shared" si="61"/>
+        <v>1102</v>
+      </c>
+      <c r="AK247" s="3">
+        <f t="shared" si="61"/>
+        <v>1117</v>
+      </c>
+      <c r="AL247" s="3">
+        <f t="shared" si="61"/>
+        <v>1093</v>
+      </c>
+      <c r="AM247" s="3">
+        <f t="shared" si="61"/>
+        <v>1041</v>
+      </c>
+      <c r="AN247" s="3">
+        <f t="shared" si="61"/>
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="248" spans="1:40">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C248" s="1"/>
+      <c r="D248" s="3">
+        <v>65079</v>
+      </c>
+      <c r="E248" s="3">
+        <v>1480</v>
+      </c>
+      <c r="F248" s="3">
+        <v>3416</v>
+      </c>
+      <c r="G248" s="3">
+        <v>3222</v>
+      </c>
+      <c r="H248" s="3">
+        <v>2927</v>
+      </c>
+      <c r="I248" s="3">
+        <v>2941</v>
+      </c>
+      <c r="J248" s="3">
+        <v>2782</v>
+      </c>
+      <c r="K248" s="3">
+        <v>2407</v>
+      </c>
+      <c r="L248" s="3">
+        <v>2335</v>
+      </c>
+      <c r="M248" s="3">
+        <v>2119</v>
+      </c>
+      <c r="N248" s="3">
+        <v>2056</v>
+      </c>
+      <c r="O248" s="3">
+        <v>1980</v>
+      </c>
+      <c r="P248" s="3">
+        <v>1946</v>
+      </c>
+      <c r="Q248" s="3">
+        <v>1948</v>
+      </c>
+      <c r="R248" s="3">
+        <v>2076</v>
+      </c>
+      <c r="S248" s="3">
+        <v>1977</v>
+      </c>
+      <c r="T248" s="3">
+        <v>2086</v>
+      </c>
+      <c r="U248" s="3">
+        <v>1888</v>
+      </c>
+      <c r="V248" s="3">
+        <v>2034</v>
+      </c>
+      <c r="W248" s="3">
+        <v>1906</v>
+      </c>
+      <c r="X248" s="3">
+        <v>1876</v>
+      </c>
+      <c r="Y248" s="3">
+        <v>1707</v>
+      </c>
+      <c r="Z248" s="3">
+        <v>1645</v>
+      </c>
+      <c r="AA248" s="3">
+        <v>1561</v>
+      </c>
+      <c r="AB248" s="3">
+        <v>1476</v>
+      </c>
+      <c r="AC248" s="3">
+        <v>1480</v>
+      </c>
+      <c r="AD248" s="3">
+        <v>1433</v>
+      </c>
+      <c r="AE248" s="3">
+        <v>1298</v>
+      </c>
+      <c r="AF248" s="3">
+        <v>1199</v>
+      </c>
+      <c r="AG248" s="3">
+        <v>1194</v>
+      </c>
+      <c r="AH248" s="3">
+        <v>1118</v>
+      </c>
+      <c r="AI248" s="3">
+        <v>1051</v>
+      </c>
+      <c r="AJ248" s="1">
+        <v>946</v>
+      </c>
+      <c r="AK248" s="1">
+        <v>960</v>
+      </c>
+      <c r="AL248" s="1">
+        <v>930</v>
+      </c>
+      <c r="AM248" s="1">
+        <v>857</v>
+      </c>
+      <c r="AN248" s="1">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="249" spans="1:40">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C249" s="1"/>
+      <c r="D249" s="3">
+        <v>7292</v>
+      </c>
+      <c r="E249" s="1">
+        <v>147</v>
+      </c>
+      <c r="F249" s="1">
+        <v>293</v>
+      </c>
+      <c r="G249" s="1">
+        <v>309</v>
+      </c>
+      <c r="H249" s="1">
+        <v>267</v>
+      </c>
+      <c r="I249" s="1">
+        <v>292</v>
+      </c>
+      <c r="J249" s="1">
+        <v>279</v>
+      </c>
+      <c r="K249" s="1">
+        <v>265</v>
+      </c>
+      <c r="L249" s="1">
+        <v>252</v>
+      </c>
+      <c r="M249" s="1">
+        <v>247</v>
+      </c>
+      <c r="N249" s="1">
+        <v>228</v>
+      </c>
+      <c r="O249" s="1">
+        <v>216</v>
+      </c>
+      <c r="P249" s="1">
+        <v>218</v>
+      </c>
+      <c r="Q249" s="1">
+        <v>216</v>
+      </c>
+      <c r="R249" s="1">
+        <v>238</v>
+      </c>
+      <c r="S249" s="1">
+        <v>214</v>
+      </c>
+      <c r="T249" s="1">
+        <v>173</v>
+      </c>
+      <c r="U249" s="1">
+        <v>195</v>
+      </c>
+      <c r="V249" s="1">
+        <v>220</v>
+      </c>
+      <c r="W249" s="1">
+        <v>215</v>
+      </c>
+      <c r="X249" s="1">
+        <v>188</v>
+      </c>
+      <c r="Y249" s="1">
+        <v>180</v>
+      </c>
+      <c r="Z249" s="1">
+        <v>202</v>
+      </c>
+      <c r="AA249" s="1">
+        <v>184</v>
+      </c>
+      <c r="AB249" s="1">
+        <v>185</v>
+      </c>
+      <c r="AC249" s="1">
+        <v>183</v>
+      </c>
+      <c r="AD249" s="1">
+        <v>135</v>
+      </c>
+      <c r="AE249" s="1">
+        <v>161</v>
+      </c>
+      <c r="AF249" s="1">
+        <v>123</v>
+      </c>
+      <c r="AG249" s="1">
+        <v>126</v>
+      </c>
+      <c r="AH249" s="1">
+        <v>118</v>
+      </c>
+      <c r="AI249" s="1">
+        <v>163</v>
+      </c>
+      <c r="AJ249" s="1">
+        <v>156</v>
+      </c>
+      <c r="AK249" s="1">
+        <v>157</v>
+      </c>
+      <c r="AL249" s="1">
+        <v>163</v>
+      </c>
+      <c r="AM249" s="1">
+        <v>184</v>
+      </c>
+      <c r="AN249" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="250" spans="1:40">
+      <c r="A250" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C250" s="1"/>
+      <c r="D250" s="3">
+        <f>SUM(D252,D251)</f>
+        <v>26155</v>
+      </c>
+      <c r="E250" s="3">
+        <f t="shared" ref="E250:AN250" si="62">SUM(E252,E251)</f>
+        <v>523</v>
+      </c>
+      <c r="F250" s="3">
+        <f t="shared" si="62"/>
+        <v>1202</v>
+      </c>
+      <c r="G250" s="3">
+        <f t="shared" si="62"/>
+        <v>1102</v>
+      </c>
+      <c r="H250" s="3">
+        <f t="shared" si="62"/>
+        <v>1050</v>
+      </c>
+      <c r="I250" s="3">
+        <f t="shared" si="62"/>
+        <v>1180</v>
+      </c>
+      <c r="J250" s="3">
+        <f t="shared" si="62"/>
+        <v>1030</v>
+      </c>
+      <c r="K250" s="3">
+        <f t="shared" si="62"/>
+        <v>968</v>
+      </c>
+      <c r="L250" s="3">
+        <f t="shared" si="62"/>
+        <v>860</v>
+      </c>
+      <c r="M250" s="3">
+        <f t="shared" si="62"/>
+        <v>954</v>
+      </c>
+      <c r="N250" s="3">
+        <f t="shared" si="62"/>
+        <v>801</v>
+      </c>
+      <c r="O250" s="3">
+        <f t="shared" si="62"/>
+        <v>815</v>
+      </c>
+      <c r="P250" s="3">
+        <f t="shared" si="62"/>
+        <v>859</v>
+      </c>
+      <c r="Q250" s="3">
+        <f t="shared" si="62"/>
+        <v>819</v>
+      </c>
+      <c r="R250" s="3">
+        <f t="shared" si="62"/>
+        <v>825</v>
+      </c>
+      <c r="S250" s="3">
+        <f t="shared" si="62"/>
+        <v>798</v>
+      </c>
+      <c r="T250" s="3">
+        <f t="shared" si="62"/>
+        <v>768</v>
+      </c>
+      <c r="U250" s="3">
+        <f t="shared" si="62"/>
+        <v>828</v>
+      </c>
+      <c r="V250" s="3">
+        <f t="shared" si="62"/>
+        <v>822</v>
+      </c>
+      <c r="W250" s="3">
+        <f t="shared" si="62"/>
+        <v>770</v>
+      </c>
+      <c r="X250" s="3">
+        <f t="shared" si="62"/>
+        <v>700</v>
+      </c>
+      <c r="Y250" s="3">
+        <f t="shared" si="62"/>
+        <v>668</v>
+      </c>
+      <c r="Z250" s="3">
+        <f t="shared" si="62"/>
+        <v>693</v>
+      </c>
+      <c r="AA250" s="3">
+        <f t="shared" si="62"/>
+        <v>667</v>
+      </c>
+      <c r="AB250" s="3">
+        <f t="shared" si="62"/>
+        <v>625</v>
+      </c>
+      <c r="AC250" s="3">
+        <f t="shared" si="62"/>
+        <v>634</v>
+      </c>
+      <c r="AD250" s="3">
+        <f t="shared" si="62"/>
+        <v>569</v>
+      </c>
+      <c r="AE250" s="3">
+        <f t="shared" si="62"/>
+        <v>526</v>
+      </c>
+      <c r="AF250" s="3">
+        <f t="shared" si="62"/>
+        <v>538</v>
+      </c>
+      <c r="AG250" s="3">
+        <f t="shared" si="62"/>
+        <v>536</v>
+      </c>
+      <c r="AH250" s="3">
+        <f t="shared" si="62"/>
+        <v>504</v>
+      </c>
+      <c r="AI250" s="3">
+        <f t="shared" si="62"/>
+        <v>426</v>
+      </c>
+      <c r="AJ250" s="3">
+        <f t="shared" si="62"/>
+        <v>457</v>
+      </c>
+      <c r="AK250" s="3">
+        <f t="shared" si="62"/>
+        <v>434</v>
+      </c>
+      <c r="AL250" s="3">
+        <f t="shared" si="62"/>
+        <v>419</v>
+      </c>
+      <c r="AM250" s="3">
+        <f t="shared" si="62"/>
+        <v>383</v>
+      </c>
+      <c r="AN250" s="3">
+        <f t="shared" si="62"/>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="251" spans="1:40">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C251" s="1"/>
+      <c r="D251" s="3">
+        <v>22896</v>
+      </c>
+      <c r="E251" s="1">
+        <v>469</v>
+      </c>
+      <c r="F251" s="3">
+        <v>1087</v>
+      </c>
+      <c r="G251" s="1">
+        <v>991</v>
+      </c>
+      <c r="H251" s="1">
+        <v>949</v>
+      </c>
+      <c r="I251" s="3">
+        <v>1052</v>
+      </c>
+      <c r="J251" s="1">
+        <v>913</v>
+      </c>
+      <c r="K251" s="1">
+        <v>865</v>
+      </c>
+      <c r="L251" s="1">
+        <v>762</v>
+      </c>
+      <c r="M251" s="1">
+        <v>850</v>
+      </c>
+      <c r="N251" s="1">
+        <v>717</v>
+      </c>
+      <c r="O251" s="1">
+        <v>730</v>
+      </c>
+      <c r="P251" s="1">
+        <v>754</v>
+      </c>
+      <c r="Q251" s="1">
+        <v>728</v>
+      </c>
+      <c r="R251" s="1">
+        <v>729</v>
+      </c>
+      <c r="S251" s="1">
+        <v>697</v>
+      </c>
+      <c r="T251" s="1">
+        <v>675</v>
+      </c>
+      <c r="U251" s="1">
+        <v>725</v>
+      </c>
+      <c r="V251" s="1">
+        <v>713</v>
+      </c>
+      <c r="W251" s="1">
+        <v>676</v>
+      </c>
+      <c r="X251" s="1">
+        <v>615</v>
+      </c>
+      <c r="Y251" s="1">
+        <v>567</v>
+      </c>
+      <c r="Z251" s="1">
+        <v>596</v>
+      </c>
+      <c r="AA251" s="1">
+        <v>585</v>
+      </c>
+      <c r="AB251" s="1">
+        <v>553</v>
+      </c>
+      <c r="AC251" s="1">
+        <v>551</v>
+      </c>
+      <c r="AD251" s="1">
+        <v>504</v>
+      </c>
+      <c r="AE251" s="1">
+        <v>463</v>
+      </c>
+      <c r="AF251" s="1">
+        <v>463</v>
+      </c>
+      <c r="AG251" s="1">
+        <v>450</v>
+      </c>
+      <c r="AH251" s="1">
+        <v>432</v>
+      </c>
+      <c r="AI251" s="1">
+        <v>366</v>
+      </c>
+      <c r="AJ251" s="1">
+        <v>382</v>
+      </c>
+      <c r="AK251" s="1">
+        <v>337</v>
+      </c>
+      <c r="AL251" s="1">
+        <v>344</v>
+      </c>
+      <c r="AM251" s="1">
+        <v>301</v>
+      </c>
+      <c r="AN251" s="1">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="252" spans="1:40">
+      <c r="A252" s="1"/>
+      <c r="B252" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C252" s="1"/>
+      <c r="D252" s="3">
+        <v>3259</v>
+      </c>
+      <c r="E252" s="1">
+        <v>54</v>
+      </c>
+      <c r="F252" s="1">
+        <v>115</v>
+      </c>
+      <c r="G252" s="1">
+        <v>111</v>
+      </c>
+      <c r="H252" s="1">
+        <v>101</v>
+      </c>
+      <c r="I252" s="1">
+        <v>128</v>
+      </c>
+      <c r="J252" s="1">
+        <v>117</v>
+      </c>
+      <c r="K252" s="1">
+        <v>103</v>
+      </c>
+      <c r="L252" s="1">
+        <v>98</v>
+      </c>
+      <c r="M252" s="1">
+        <v>104</v>
+      </c>
+      <c r="N252" s="1">
+        <v>84</v>
+      </c>
+      <c r="O252" s="1">
+        <v>85</v>
+      </c>
+      <c r="P252" s="1">
+        <v>105</v>
+      </c>
+      <c r="Q252" s="1">
+        <v>91</v>
+      </c>
+      <c r="R252" s="1">
+        <v>96</v>
+      </c>
+      <c r="S252" s="1">
+        <v>101</v>
+      </c>
+      <c r="T252" s="1">
+        <v>93</v>
+      </c>
+      <c r="U252" s="1">
+        <v>103</v>
+      </c>
+      <c r="V252" s="1">
+        <v>109</v>
+      </c>
+      <c r="W252" s="1">
+        <v>94</v>
+      </c>
+      <c r="X252" s="1">
+        <v>85</v>
+      </c>
+      <c r="Y252" s="1">
+        <v>101</v>
+      </c>
+      <c r="Z252" s="1">
+        <v>97</v>
+      </c>
+      <c r="AA252" s="1">
+        <v>82</v>
+      </c>
+      <c r="AB252" s="1">
+        <v>72</v>
+      </c>
+      <c r="AC252" s="1">
+        <v>83</v>
+      </c>
+      <c r="AD252" s="1">
+        <v>65</v>
+      </c>
+      <c r="AE252" s="1">
+        <v>63</v>
+      </c>
+      <c r="AF252" s="1">
+        <v>75</v>
+      </c>
+      <c r="AG252" s="1">
+        <v>86</v>
+      </c>
+      <c r="AH252" s="1">
+        <v>72</v>
+      </c>
+      <c r="AI252" s="1">
+        <v>60</v>
+      </c>
+      <c r="AJ252" s="1">
+        <v>75</v>
+      </c>
+      <c r="AK252" s="1">
+        <v>97</v>
+      </c>
+      <c r="AL252" s="1">
+        <v>75</v>
+      </c>
+      <c r="AM252" s="1">
+        <v>82</v>
+      </c>
+      <c r="AN252" s="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="256" spans="1:40">
+      <c r="A256" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B256" s="16"/>
+      <c r="C256" s="16"/>
+      <c r="D256" s="16"/>
+      <c r="E256" s="16"/>
+      <c r="F256" s="16"/>
+      <c r="G256" s="16"/>
+      <c r="H256" s="16"/>
+      <c r="I256" s="16"/>
+      <c r="J256" s="13"/>
+    </row>
+    <row r="257" spans="1:10">
+      <c r="A257" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B257" s="22"/>
+      <c r="C257" s="22"/>
+      <c r="D257" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G257" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H257" s="22"/>
+      <c r="I257" s="22"/>
+      <c r="J257" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10">
+      <c r="A258" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C258" s="1"/>
+      <c r="D258" s="4">
+        <f>AVERAGE(L238:Q238)</f>
+        <v>17374.166666666668</v>
+      </c>
+      <c r="E258" s="4"/>
+      <c r="G258" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H258" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I258" s="1"/>
+      <c r="J258">
+        <f>J259+J260</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10">
+      <c r="A259" s="1"/>
+      <c r="B259" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C259" s="1"/>
+      <c r="D259" s="4">
+        <f>AVERAGE(L239:Q239)</f>
+        <v>15288.166666666666</v>
+      </c>
+      <c r="G259" s="1"/>
+      <c r="H259" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I259" s="1"/>
+      <c r="J259">
+        <f>D259/D258</f>
+        <v>0.87993668761091648</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10">
+      <c r="A260" s="1"/>
+      <c r="B260" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C260" s="1"/>
+      <c r="D260" s="4">
+        <f>AVERAGE(L240:Q240)</f>
+        <v>2086</v>
+      </c>
+      <c r="G260" s="1"/>
+      <c r="H260" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I260" s="1"/>
+      <c r="J260">
+        <f>D260/D258</f>
+        <v>0.1200633123890834</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="19">
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="A257:C257"/>
+    <mergeCell ref="A112:L112"/>
+    <mergeCell ref="G257:I257"/>
+    <mergeCell ref="A256:J256"/>
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="I65:J65"/>
     <mergeCell ref="K87:L87"/>
-    <mergeCell ref="A87:B87"/>
     <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A87:D87"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
@@ -19113,7 +21404,6 @@
     <mergeCell ref="A171:B171"/>
     <mergeCell ref="A205:B205"/>
     <mergeCell ref="I113:J113"/>
-    <mergeCell ref="A112:B112"/>
     <mergeCell ref="A137:B137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>